<commit_message>
Waarderingskamer: minimum config compleet
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -861,12 +861,6 @@
     <t>BSM: opleveren</t>
   </si>
   <si>
-    <t>k.boersma@ihw.nl</t>
-  </si>
-  <si>
-    <t>https://www.ihw.nl</t>
-  </si>
-  <si>
     <t>SIM</t>
   </si>
   <si>
@@ -946,6 +940,12 @@
   </si>
   <si>
     <t>https://waarderingskamer.github.io/[model-abbreviation]/</t>
+  </si>
+  <si>
+    <t>r.kathmann@waarderingskamer.nl</t>
+  </si>
+  <si>
+    <t>https://www.waarderingskamer.nl/</t>
   </si>
 </sst>
 </file>
@@ -1516,10 +1516,10 @@
   <dimension ref="A1:P132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S17" sqref="S17"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1589,10 +1589,10 @@
       <c r="F2" s="3"/>
       <c r="G2" s="19"/>
       <c r="H2" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>274</v>
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G18" s="20"/>
       <c r="K18" s="20"/>
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="G20" s="20"/>
       <c r="K20" s="20"/>
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="G21" s="20"/>
       <c r="K21" s="20"/>
@@ -2382,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="31"/>
@@ -2390,13 +2390,13 @@
       <c r="J30" s="32"/>
       <c r="K30" s="27"/>
       <c r="L30" s="38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M30" s="45" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N30" s="45" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O30" s="27"/>
       <c r="P30"/>
@@ -2549,13 +2549,13 @@
     </row>
     <row r="36" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="40" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B36" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D36" s="40" t="b">
         <v>0</v>
@@ -2668,27 +2668,27 @@
         <v>1</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G40" s="27"/>
       <c r="H40" s="36" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I40" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J40" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K40" s="27"/>
       <c r="L40" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M40" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N40" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O40" s="27"/>
       <c r="P40"/>
@@ -2909,23 +2909,23 @@
       </c>
       <c r="G49" s="21"/>
       <c r="H49" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I49" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J49" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K49" s="21"/>
       <c r="L49" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M49" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N49" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O49" s="21"/>
       <c r="P49"/>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="56" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A56" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D56" s="16" t="b">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="16"/>
@@ -3113,22 +3113,22 @@
     </row>
     <row r="57" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>293</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>295</v>
       </c>
       <c r="G57" s="27"/>
       <c r="K57" s="27"/>
@@ -3136,13 +3136,13 @@
     </row>
     <row r="58" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D58" s="7" t="b">
         <v>0</v>
@@ -3151,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G58" s="27"/>
       <c r="H58" s="34"/>
@@ -3354,7 +3354,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G66" s="20"/>
       <c r="K66" s="20"/>
@@ -3436,23 +3436,23 @@
       </c>
       <c r="G69" s="20"/>
       <c r="H69" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J69" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K69" s="21"/>
       <c r="L69" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M69" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N69" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O69" s="27"/>
       <c r="P69"/>
@@ -3465,7 +3465,7 @@
         <v>10</v>
       </c>
       <c r="C70" s="46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D70" s="46" t="b">
         <v>0</v>
@@ -3579,23 +3579,23 @@
       <c r="F74" s="33"/>
       <c r="G74" s="20"/>
       <c r="H74" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I74" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J74" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K74" s="21"/>
       <c r="L74" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M74" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N74" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O74" s="27"/>
       <c r="P74"/>
@@ -3644,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G76" s="20"/>
       <c r="K76" s="20"/>
@@ -3720,23 +3720,23 @@
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J79" s="17" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K79" s="20"/>
       <c r="L79" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M79" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N79" s="38" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="O79" s="27"/>
       <c r="P79"/>
@@ -3999,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G89" s="20"/>
       <c r="I89" s="35"/>
@@ -4040,13 +4040,13 @@
     </row>
     <row r="91" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -4055,7 +4055,7 @@
         <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G91" s="27"/>
       <c r="K91" s="27"/>
@@ -4078,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G92" s="20"/>
       <c r="K92" s="20"/>
@@ -4184,23 +4184,23 @@
       </c>
       <c r="G96" s="20"/>
       <c r="H96" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I96" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J96" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K96" s="21"/>
       <c r="L96" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M96" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N96" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O96" s="27"/>
       <c r="P96"/>
@@ -4426,13 +4426,13 @@
     </row>
     <row r="104" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B104" t="s">
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -4569,7 +4569,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="47" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G108" s="20"/>
       <c r="K108" s="20"/>

</xml_diff>

<commit_message>
[Waarderingskamer] toolbox EA toegevoegd, naam = WKMIM
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -964,6 +964,12 @@
   </si>
   <si>
     <t>Yes if scalar types may be entered without reference to a UML datatype</t>
+  </si>
+  <si>
+    <t>createeatoolbox</t>
+  </si>
+  <si>
+    <t>Should an EA toolbox be generated?</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1114,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1219,6 +1225,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1537,13 +1546,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q134"/>
+  <dimension ref="A1:Q135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A72" sqref="A72:XFD72"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1734,16 +1743,16 @@
       <c r="P6"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50" t="b">
+      <c r="D7" s="51" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1758,10 +1767,10 @@
       <c r="P7"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
       <c r="G8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="38"/>
@@ -2282,40 +2291,40 @@
       <c r="O26" s="27"/>
       <c r="P26"/>
     </row>
-    <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="1:16" s="50" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="50" t="s">
+        <v>313</v>
+      </c>
+      <c r="B27" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="38" t="s">
+      <c r="C27" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="D27" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="27"/>
+      <c r="L27" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="N27" s="50" t="s">
         <v>4</v>
       </c>
       <c r="O27" s="27"/>
@@ -2323,16 +2332,16 @@
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -2342,7 +2351,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>4</v>
@@ -2352,7 +2361,7 @@
         <v>16</v>
       </c>
       <c r="M28" s="38" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N28" s="38" t="s">
         <v>4</v>
@@ -2360,119 +2369,119 @@
       <c r="O28" s="27"/>
       <c r="P28"/>
     </row>
-    <row r="29" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="D29" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="27"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
+      <c r="C29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="20"/>
+      <c r="L29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O29" s="27"/>
       <c r="P29"/>
     </row>
-    <row r="30" spans="1:16" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D30" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>296</v>
+    <row r="30" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D30" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="G30" s="27"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
       <c r="K30" s="27"/>
-      <c r="L30" s="38" t="s">
-        <v>301</v>
-      </c>
-      <c r="M30" s="45" t="s">
-        <v>301</v>
-      </c>
-      <c r="N30" s="45" t="s">
-        <v>301</v>
-      </c>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
       <c r="O30" s="27"/>
       <c r="P30"/>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="20"/>
-      <c r="L31" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="N31" s="42" t="s">
-        <v>19</v>
+    <row r="31" spans="1:16" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="D31" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="M31" s="45" t="s">
+        <v>301</v>
+      </c>
+      <c r="N31" s="45" t="s">
+        <v>301</v>
       </c>
       <c r="O31" s="27"/>
       <c r="P31"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
@@ -2480,26 +2489,38 @@
       <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G32" s="20"/>
+      <c r="H32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>34</v>
+      </c>
       <c r="K32" s="20"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
+      <c r="L32" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="N32" s="42" t="s">
+        <v>19</v>
+      </c>
       <c r="O32" s="27"/>
       <c r="P32"/>
     </row>
-    <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2508,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>268</v>
+        <v>10</v>
       </c>
       <c r="G33" s="20"/>
       <c r="K33" s="20"/>
@@ -2518,124 +2539,124 @@
       <c r="O33" s="27"/>
       <c r="P33"/>
     </row>
-    <row r="34" spans="1:16" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>272</v>
-      </c>
-      <c r="D34" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="G34" s="27"/>
-      <c r="K34" s="27"/>
+    <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="38"/>
       <c r="M34" s="38"/>
       <c r="N34" s="38"/>
       <c r="O34" s="27"/>
-    </row>
-    <row r="35" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="P34"/>
+    </row>
+    <row r="35" spans="1:16" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="D35" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="G35" s="27"/>
+      <c r="K35" s="27"/>
       <c r="L35" s="38"/>
       <c r="M35" s="38"/>
       <c r="N35" s="38"/>
       <c r="O35" s="27"/>
-      <c r="P35"/>
-    </row>
-    <row r="36" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="40" t="s">
+    </row>
+    <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="27"/>
+      <c r="P36"/>
+    </row>
+    <row r="37" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="40" t="s">
         <v>282</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B37" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C37" s="40" t="s">
         <v>283</v>
       </c>
-      <c r="D36" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="O36" s="41"/>
-    </row>
-    <row r="37" spans="1:16" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+      <c r="D37" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="O37" s="41"/>
+    </row>
+    <row r="38" spans="1:16" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="27"/>
-      <c r="P37"/>
-    </row>
-    <row r="38" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>16</v>
@@ -2648,21 +2669,21 @@
       <c r="O38" s="27"/>
       <c r="P38"/>
     </row>
-    <row r="39" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>16</v>
@@ -2675,120 +2696,123 @@
       <c r="O39" s="27"/>
       <c r="P39"/>
     </row>
-    <row r="40" spans="1:16" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A40" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="D40" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="30" t="s">
-        <v>296</v>
-      </c>
-      <c r="G40" s="27"/>
-      <c r="H40" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="I40" s="39" t="s">
-        <v>302</v>
-      </c>
-      <c r="J40" s="39" t="s">
-        <v>302</v>
-      </c>
-      <c r="K40" s="27"/>
-      <c r="L40" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M40" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N40" s="47" t="s">
-        <v>301</v>
-      </c>
+    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
       <c r="O40" s="27"/>
       <c r="P40"/>
     </row>
-    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="K41" s="20"/>
-      <c r="L41" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N41" s="38" t="s">
-        <v>4</v>
+    <row r="41" spans="1:16" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="D41" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="G41" s="27"/>
+      <c r="H41" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="I41" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="J41" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="K41" s="27"/>
+      <c r="L41" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N41" s="47" t="s">
+        <v>301</v>
       </c>
       <c r="O41" s="27"/>
       <c r="P41"/>
     </row>
-    <row r="42" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A42" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="7" t="s">
+    <row r="42" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>16</v>
+      <c r="C42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G42" s="20"/>
+      <c r="H42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="43" t="s">
+        <v>16</v>
+      </c>
       <c r="K42" s="20"/>
+      <c r="L42" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O42" s="27"/>
       <c r="P42"/>
     </row>
-    <row r="43" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D43" s="7" t="b">
         <v>1</v>
@@ -2797,45 +2821,56 @@
         <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>218</v>
+        <v>16</v>
       </c>
       <c r="G43" s="20"/>
       <c r="K43" s="20"/>
       <c r="O43" s="27"/>
       <c r="P43"/>
     </row>
-    <row r="44" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>16</v>
+    <row r="44" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="G44" s="20"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
       <c r="O44" s="27"/>
       <c r="P44"/>
     </row>
     <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="50"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
+      <c r="A45" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G45" s="20"/>
       <c r="K45" s="20"/>
       <c r="L45" s="38"/>
@@ -2844,22 +2879,11 @@
       <c r="O45" s="27"/>
       <c r="P45"/>
     </row>
-    <row r="46" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="51"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
       <c r="G46" s="20"/>
       <c r="K46" s="20"/>
       <c r="L46" s="38"/>
@@ -2868,21 +2892,21 @@
       <c r="O46" s="27"/>
       <c r="P46"/>
     </row>
-    <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
+        <v>177</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="20"/>
       <c r="K47" s="20"/>
@@ -2892,15 +2916,15 @@
       <c r="O47" s="27"/>
       <c r="P47"/>
     </row>
-    <row r="48" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
@@ -2908,86 +2932,86 @@
       <c r="E48" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G48" s="21"/>
-      <c r="K48" s="21"/>
+      <c r="G48" s="20"/>
+      <c r="K48" s="20"/>
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" s="38"/>
-      <c r="O48" s="21"/>
+      <c r="O48" s="27"/>
       <c r="P48"/>
     </row>
     <row r="49" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D49" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="G49" s="21"/>
-      <c r="H49" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I49" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J49" s="47" t="s">
-        <v>302</v>
-      </c>
       <c r="K49" s="21"/>
-      <c r="L49" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M49" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N49" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="38"/>
       <c r="O49" s="21"/>
       <c r="P49"/>
     </row>
-    <row r="50" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I50" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J50" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K50" s="21"/>
+      <c r="L50" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M50" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N50" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="O50" s="21"/>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="O50" s="27"/>
-      <c r="P50"/>
-    </row>
-    <row r="51" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>183</v>
-      </c>
       <c r="D51" s="7" t="b">
         <v>0</v>
       </c>
@@ -2995,49 +3019,46 @@
         <v>1</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>209</v>
+        <v>4</v>
       </c>
       <c r="G51" s="20"/>
       <c r="K51" s="20"/>
       <c r="O51" s="27"/>
       <c r="P51"/>
     </row>
-    <row r="52" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>16</v>
+    <row r="52" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="G52" s="20"/>
       <c r="K52" s="20"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="38"/>
       <c r="O52" s="27"/>
       <c r="P52"/>
     </row>
     <row r="53" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D53" s="2" t="b">
         <v>0</v>
@@ -3056,320 +3077,320 @@
       <c r="O53" s="27"/>
       <c r="P53"/>
     </row>
-    <row r="54" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="7" t="s">
+    <row r="54" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="20"/>
       <c r="K54" s="20"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="38"/>
+      <c r="N54" s="38"/>
       <c r="O54" s="27"/>
       <c r="P54"/>
     </row>
-    <row r="55" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B55" s="2" t="s">
+    <row r="55" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="C55" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="20"/>
       <c r="K55" s="20"/>
-      <c r="L55" s="38"/>
-      <c r="M55" s="38"/>
-      <c r="N55" s="38"/>
       <c r="O55" s="27"/>
       <c r="P55"/>
     </row>
-    <row r="56" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A56" s="16" t="s">
+    <row r="56" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="27"/>
+      <c r="P56"/>
+    </row>
+    <row r="57" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B57" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C57" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="D56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="16" t="s">
+      <c r="D57" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G56" s="22"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="16"/>
-      <c r="O56" s="22"/>
-      <c r="P56"/>
-    </row>
-    <row r="57" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+      <c r="G57" s="22"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="22"/>
+      <c r="L57" s="16"/>
+      <c r="O57" s="22"/>
+      <c r="P57"/>
+    </row>
+    <row r="58" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="G57" s="27"/>
-      <c r="K57" s="27"/>
-      <c r="O57" s="27"/>
-    </row>
-    <row r="58" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>304</v>
-      </c>
       <c r="G58" s="27"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
       <c r="K58" s="27"/>
       <c r="O58" s="27"/>
     </row>
     <row r="59" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="G59" s="27"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="27"/>
+      <c r="O59" s="27"/>
+    </row>
+    <row r="60" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" s="20"/>
-      <c r="K59" s="20"/>
-      <c r="O59" s="27"/>
-      <c r="P59"/>
-    </row>
-    <row r="60" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="16" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="O60" s="27"/>
+      <c r="P60"/>
+    </row>
+    <row r="61" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B61" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D60" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="16" t="s">
+      <c r="D61" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="G60" s="22"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="16"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="16"/>
-      <c r="O60" s="22"/>
-      <c r="P60"/>
-    </row>
-    <row r="61" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
+      <c r="G61" s="22"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="22"/>
+      <c r="P61"/>
+    </row>
+    <row r="62" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G61" s="20"/>
-      <c r="K61" s="20"/>
-      <c r="O61" s="27"/>
-      <c r="P61"/>
-    </row>
-    <row r="62" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G62" s="20"/>
       <c r="K62" s="20"/>
-      <c r="L62" s="38"/>
-      <c r="M62" s="38"/>
-      <c r="N62" s="38"/>
       <c r="O62" s="27"/>
       <c r="P62"/>
     </row>
-    <row r="63" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D63" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>218</v>
+    <row r="63" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="G63" s="20"/>
       <c r="K63" s="20"/>
+      <c r="L63" s="38"/>
+      <c r="M63" s="38"/>
+      <c r="N63" s="38"/>
       <c r="O63" s="27"/>
       <c r="P63"/>
     </row>
     <row r="64" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>261</v>
-      </c>
-      <c r="B64" t="s">
-        <v>81</v>
-      </c>
-      <c r="C64" t="s">
-        <v>262</v>
-      </c>
-      <c r="D64" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>226</v>
-      </c>
-      <c r="G64" s="27"/>
-      <c r="K64" s="27"/>
+      <c r="A64" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G64" s="20"/>
+      <c r="K64" s="20"/>
       <c r="O64" s="27"/>
       <c r="P64"/>
     </row>
-    <row r="65" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="38"/>
+    <row r="65" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>226</v>
+      </c>
+      <c r="G65" s="27"/>
+      <c r="K65" s="27"/>
       <c r="O65" s="27"/>
       <c r="P65"/>
     </row>
     <row r="66" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>0</v>
@@ -3378,7 +3399,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>300</v>
+        <v>210</v>
       </c>
       <c r="G66" s="20"/>
       <c r="K66" s="20"/>
@@ -3390,22 +3411,22 @@
     </row>
     <row r="67" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>208</v>
+        <v>300</v>
       </c>
       <c r="G67" s="20"/>
       <c r="K67" s="20"/>
@@ -3415,24 +3436,24 @@
       <c r="O67" s="27"/>
       <c r="P67"/>
     </row>
-    <row r="68" spans="1:17" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="D68" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>254</v>
+    <row r="68" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="G68" s="20"/>
       <c r="K68" s="20"/>
@@ -3442,162 +3463,162 @@
       <c r="O68" s="27"/>
       <c r="P68"/>
     </row>
-    <row r="69" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D69" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
+    <row r="69" spans="1:17" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D69" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>254</v>
       </c>
       <c r="G69" s="20"/>
-      <c r="H69" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I69" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J69" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K69" s="21"/>
-      <c r="L69" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M69" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N69" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K69" s="20"/>
+      <c r="L69" s="38"/>
+      <c r="M69" s="38"/>
+      <c r="N69" s="38"/>
       <c r="O69" s="27"/>
       <c r="P69"/>
     </row>
     <row r="70" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="B70" s="46" t="s">
+      <c r="A70" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="46" t="s">
-        <v>297</v>
-      </c>
-      <c r="D70" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="46"/>
+      <c r="C70" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="G70" s="20"/>
-      <c r="K70" s="20"/>
-      <c r="L70" s="38"/>
-      <c r="M70" s="38"/>
-      <c r="N70" s="38"/>
+      <c r="H70" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I70" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J70" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K70" s="21"/>
+      <c r="L70" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M70" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N70" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O70" s="27"/>
       <c r="P70"/>
     </row>
-    <row r="71" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D71" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>4</v>
-      </c>
+    <row r="71" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="46" t="s">
+        <v>297</v>
+      </c>
+      <c r="D71" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="46"/>
       <c r="G71" s="20"/>
       <c r="K71" s="20"/>
+      <c r="L71" s="38"/>
+      <c r="M71" s="38"/>
+      <c r="N71" s="38"/>
       <c r="O71" s="27"/>
       <c r="P71"/>
     </row>
-    <row r="72" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="40" t="s">
+    <row r="72" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="O72" s="27"/>
+      <c r="P72"/>
+    </row>
+    <row r="73" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="B72" s="40" t="s">
+      <c r="B73" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="40" t="s">
+      <c r="C73" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="D72" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="G72" s="27"/>
-      <c r="L72" s="27"/>
-      <c r="Q72" s="27"/>
-    </row>
-    <row r="73" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="20"/>
-      <c r="K73" s="20"/>
-      <c r="L73" s="38"/>
-      <c r="M73" s="38"/>
-      <c r="N73" s="38"/>
-      <c r="O73" s="27"/>
-      <c r="P73"/>
+      <c r="D73" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="27"/>
+      <c r="L73" s="27"/>
+      <c r="Q73" s="27"/>
     </row>
     <row r="74" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>77</v>
+        <v>229</v>
       </c>
       <c r="D74" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G74" s="20"/>
       <c r="K74" s="20"/>
@@ -3609,421 +3630,421 @@
     </row>
     <row r="75" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D75" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F75" s="33"/>
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G75" s="20"/>
-      <c r="H75" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I75" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J75" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K75" s="21"/>
-      <c r="L75" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M75" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N75" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K75" s="20"/>
+      <c r="L75" s="38"/>
+      <c r="M75" s="38"/>
+      <c r="N75" s="38"/>
       <c r="O75" s="27"/>
       <c r="P75"/>
     </row>
     <row r="76" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D76" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>269</v>
-      </c>
+      <c r="F76" s="33"/>
       <c r="G76" s="20"/>
-      <c r="K76" s="20"/>
-      <c r="L76" s="38"/>
-      <c r="M76" s="38"/>
-      <c r="N76" s="38"/>
+      <c r="H76" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I76" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J76" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K76" s="21"/>
+      <c r="L76" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M76" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N76" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O76" s="27"/>
       <c r="P76"/>
     </row>
-    <row r="77" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>298</v>
+    <row r="77" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="G77" s="20"/>
       <c r="K77" s="20"/>
+      <c r="L77" s="38"/>
+      <c r="M77" s="38"/>
+      <c r="N77" s="38"/>
       <c r="O77" s="27"/>
       <c r="P77"/>
     </row>
-    <row r="78" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>19</v>
+    <row r="78" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>298</v>
       </c>
       <c r="G78" s="20"/>
       <c r="K78" s="20"/>
-      <c r="L78" s="38"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="38"/>
       <c r="O78" s="27"/>
       <c r="P78"/>
     </row>
-    <row r="79" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>211</v>
+    <row r="79" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G79" s="20"/>
       <c r="K79" s="20"/>
+      <c r="L79" s="38"/>
+      <c r="M79" s="38"/>
+      <c r="N79" s="38"/>
       <c r="O79" s="27"/>
       <c r="P79"/>
     </row>
-    <row r="80" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
+    <row r="80" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="G80" s="20"/>
-      <c r="H80" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>278</v>
-      </c>
       <c r="K80" s="20"/>
-      <c r="L80" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="M80" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="N80" s="38" t="s">
-        <v>279</v>
-      </c>
       <c r="O80" s="27"/>
       <c r="P80"/>
     </row>
     <row r="81" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D81" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G81" s="20"/>
+      <c r="H81" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J81" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="K81" s="20"/>
-      <c r="L81" s="38"/>
-      <c r="M81" s="38"/>
-      <c r="N81" s="38"/>
+      <c r="L81" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="M81" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="N81" s="38" t="s">
+        <v>279</v>
+      </c>
       <c r="O81" s="27"/>
       <c r="P81"/>
     </row>
-    <row r="82" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>92</v>
+    <row r="82" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="G82" s="20"/>
       <c r="K82" s="20"/>
+      <c r="L82" s="38"/>
+      <c r="M82" s="38"/>
+      <c r="N82" s="38"/>
       <c r="O82" s="27"/>
       <c r="P82"/>
     </row>
     <row r="83" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D83" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="G83" s="20"/>
       <c r="K83" s="20"/>
       <c r="O83" s="27"/>
       <c r="P83"/>
     </row>
-    <row r="84" spans="1:16" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>96</v>
+    <row r="84" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G84" s="20"/>
       <c r="K84" s="20"/>
-      <c r="L84" s="38"/>
-      <c r="M84" s="38"/>
-      <c r="N84" s="38"/>
       <c r="O84" s="27"/>
       <c r="P84"/>
     </row>
-    <row r="85" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:16" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D85" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G85" s="20"/>
-      <c r="H85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K85" s="20"/>
-      <c r="L85" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M85" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N85" s="38" t="s">
-        <v>4</v>
-      </c>
+      <c r="L85" s="38"/>
+      <c r="M85" s="38"/>
+      <c r="N85" s="38"/>
       <c r="O85" s="27"/>
       <c r="P85"/>
     </row>
     <row r="86" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
       <c r="D86" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G86" s="20"/>
+      <c r="H86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="K86" s="20"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="38"/>
+      <c r="L86" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M86" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O86" s="27"/>
       <c r="P86"/>
     </row>
-    <row r="87" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D87" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="G87" s="27"/>
-      <c r="K87" s="27"/>
+    <row r="87" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="20"/>
+      <c r="K87" s="20"/>
       <c r="L87" s="38"/>
       <c r="M87" s="38"/>
       <c r="N87" s="38"/>
       <c r="O87" s="27"/>
       <c r="P87"/>
     </row>
-    <row r="88" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="G88" s="20"/>
-      <c r="K88" s="20"/>
+    <row r="88" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B88" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="G88" s="27"/>
+      <c r="K88" s="27"/>
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
       <c r="N88" s="38"/>
       <c r="O88" s="27"/>
       <c r="P88"/>
     </row>
-    <row r="89" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="D89" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>250</v>
+    <row r="89" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="12" t="s">
+        <v>251</v>
       </c>
       <c r="G89" s="20"/>
       <c r="K89" s="20"/>
@@ -4033,24 +4054,26 @@
       <c r="O89" s="27"/>
       <c r="P89"/>
     </row>
-    <row r="90" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>298</v>
+    <row r="90" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="G90" s="20"/>
-      <c r="I90" s="35"/>
-      <c r="J90" s="35"/>
       <c r="K90" s="20"/>
       <c r="L90" s="38"/>
       <c r="M90" s="38"/>
@@ -4058,26 +4081,24 @@
       <c r="O90" s="27"/>
       <c r="P90"/>
     </row>
-    <row r="91" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F91" s="2" t="s">
-        <v>16</v>
+      <c r="F91" s="17" t="s">
+        <v>298</v>
       </c>
       <c r="G91" s="20"/>
+      <c r="I91" s="35"/>
+      <c r="J91" s="35"/>
       <c r="K91" s="20"/>
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
@@ -4085,65 +4106,65 @@
       <c r="O91" s="27"/>
       <c r="P91"/>
     </row>
-    <row r="92" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
+    <row r="92" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="20"/>
+      <c r="K92" s="20"/>
+      <c r="L92" s="38"/>
+      <c r="M92" s="38"/>
+      <c r="N92" s="38"/>
+      <c r="O92" s="27"/>
+      <c r="P92"/>
+    </row>
+    <row r="93" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
         <v>284</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>10</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>285</v>
       </c>
-      <c r="D92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="D93" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
         <v>298</v>
       </c>
-      <c r="G92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="O92" s="27"/>
-    </row>
-    <row r="93" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G93" s="20"/>
-      <c r="K93" s="20"/>
-      <c r="L93" s="38"/>
-      <c r="M93" s="38"/>
-      <c r="N93" s="38"/>
+      <c r="G93" s="27"/>
+      <c r="K93" s="27"/>
       <c r="O93" s="27"/>
-      <c r="P93"/>
     </row>
     <row r="94" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D94" s="2" t="b">
         <v>0</v>
@@ -4151,8 +4172,8 @@
       <c r="E94" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F94" s="2" t="s">
-        <v>16</v>
+      <c r="F94" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="G94" s="20"/>
       <c r="K94" s="20"/>
@@ -4162,21 +4183,24 @@
       <c r="O94" s="27"/>
       <c r="P94"/>
     </row>
-    <row r="95" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G95" s="20"/>
       <c r="K95" s="20"/>
@@ -4188,22 +4212,19 @@
     </row>
     <row r="96" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="G96" s="20"/>
       <c r="K96" s="20"/>
@@ -4213,15 +4234,15 @@
       <c r="O96" s="27"/>
       <c r="P96"/>
     </row>
-    <row r="97" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>1</v>
@@ -4229,62 +4250,65 @@
       <c r="E97" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F97" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G97" s="20"/>
-      <c r="H97" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I97" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J97" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K97" s="21"/>
-      <c r="L97" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M97" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N97" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K97" s="20"/>
+      <c r="L97" s="38"/>
+      <c r="M97" s="38"/>
+      <c r="N97" s="38"/>
       <c r="O97" s="27"/>
       <c r="P97"/>
     </row>
-    <row r="98" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>218</v>
+    <row r="98" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G98" s="20"/>
-      <c r="K98" s="20"/>
+      <c r="H98" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I98" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J98" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K98" s="21"/>
+      <c r="L98" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M98" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N98" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O98" s="27"/>
       <c r="P98"/>
     </row>
     <row r="99" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D99" s="7" t="b">
         <v>1</v>
@@ -4302,79 +4326,64 @@
     </row>
     <row r="100" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D100" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E100" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="G100" s="20"/>
       <c r="K100" s="20"/>
       <c r="O100" s="27"/>
       <c r="P100"/>
     </row>
-    <row r="101" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B101" s="2" t="s">
+    <row r="101" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B101" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
+      <c r="C101" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G101" s="20"/>
-      <c r="H101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K101" s="20"/>
-      <c r="L101" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="M101" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N101" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="O101" s="27"/>
       <c r="P101"/>
     </row>
     <row r="102" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
         <v>1</v>
@@ -4404,23 +4413,23 @@
     </row>
     <row r="103" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D103" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G103" s="20"/>
       <c r="H103" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>4</v>
@@ -4430,7 +4439,7 @@
       </c>
       <c r="K103" s="20"/>
       <c r="L103" s="38" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="M103" s="38" t="s">
         <v>4</v>
@@ -4441,15 +4450,15 @@
       <c r="O103" s="27"/>
       <c r="P103"/>
     </row>
-    <row r="104" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>0</v>
@@ -4457,119 +4466,120 @@
       <c r="E104" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F104" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G104" s="20"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
+      <c r="H104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="K104" s="20"/>
-      <c r="L104" s="38"/>
-      <c r="M104" s="38"/>
-      <c r="N104" s="38"/>
+      <c r="L104" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M104" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N104" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O104" s="27"/>
       <c r="P104"/>
     </row>
-    <row r="105" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>286</v>
-      </c>
-      <c r="B105" t="s">
+    <row r="105" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C105" t="s">
-        <v>287</v>
-      </c>
-      <c r="D105" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" t="s">
-        <v>4</v>
-      </c>
-      <c r="G105" s="27"/>
+      <c r="C105" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" s="20"/>
       <c r="H105"/>
       <c r="I105"/>
       <c r="J105"/>
-      <c r="K105" s="27"/>
-      <c r="L105"/>
-      <c r="M105"/>
-      <c r="N105"/>
+      <c r="K105" s="20"/>
+      <c r="L105" s="38"/>
+      <c r="M105" s="38"/>
+      <c r="N105" s="38"/>
       <c r="O105" s="27"/>
-    </row>
-    <row r="106" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A106" s="7" t="s">
+      <c r="P105"/>
+    </row>
+    <row r="106" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>286</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>287</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="27"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106" s="27"/>
+      <c r="L106"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106" s="27"/>
+    </row>
+    <row r="107" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B107" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" s="20"/>
-      <c r="K106" s="20"/>
-      <c r="O106" s="27"/>
-    </row>
-    <row r="107" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
+      <c r="D107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G107" s="20"/>
-      <c r="H107" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K107" s="20"/>
-      <c r="L107" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N107" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="O107" s="27"/>
     </row>
     <row r="108" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>1</v>
@@ -4601,169 +4611,204 @@
     </row>
     <row r="109" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="20"/>
+      <c r="H109" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="20"/>
+      <c r="L109" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M109" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N109" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="O109" s="27"/>
+    </row>
+    <row r="110" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F109" s="47" t="s">
+      <c r="D110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="47" t="s">
         <v>298</v>
       </c>
-      <c r="G109" s="20"/>
-      <c r="K109" s="20"/>
-      <c r="L109" s="38"/>
-      <c r="M109" s="38"/>
-      <c r="N109" s="38"/>
-      <c r="O109" s="27"/>
-    </row>
-    <row r="110" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="48" t="s">
+      <c r="G110" s="20"/>
+      <c r="K110" s="20"/>
+      <c r="L110" s="38"/>
+      <c r="M110" s="38"/>
+      <c r="N110" s="38"/>
+      <c r="O110" s="27"/>
+    </row>
+    <row r="111" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="B110" s="48" t="s">
+      <c r="B111" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C110" s="48" t="s">
+      <c r="C111" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="D110" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="G110" s="27"/>
-      <c r="H110" s="48" t="s">
+      <c r="D111" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="27"/>
+      <c r="H111" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="I110" s="48" t="s">
+      <c r="I111" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="J110" s="48" t="s">
+      <c r="J111" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="K110" s="21"/>
-      <c r="L110" s="48" t="s">
+      <c r="K111" s="21"/>
+      <c r="L111" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="M110" s="48" t="s">
+      <c r="M111" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="N110" s="48" t="s">
+      <c r="N111" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="O110" s="27"/>
-    </row>
-    <row r="111" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A111" s="26" t="s">
+      <c r="O111" s="27"/>
+    </row>
+    <row r="112" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A112" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B112" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C111" s="26" t="s">
+      <c r="C112" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="D111" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="26" t="s">
+      <c r="D112" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="G111" s="27"/>
-      <c r="H111" s="26"/>
-      <c r="I111" s="26"/>
-      <c r="J111" s="26"/>
-      <c r="K111" s="27"/>
-      <c r="L111" s="38"/>
-      <c r="M111" s="38"/>
-      <c r="N111" s="38"/>
-      <c r="O111" s="27"/>
-    </row>
-    <row r="112" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G112" s="20"/>
-      <c r="K112" s="20"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="26"/>
+      <c r="I112" s="26"/>
+      <c r="J112" s="26"/>
+      <c r="K112" s="27"/>
       <c r="L112" s="38"/>
       <c r="M112" s="38"/>
       <c r="N112" s="38"/>
       <c r="O112" s="27"/>
     </row>
-    <row r="113" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P113"/>
-    </row>
-    <row r="114" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G113" s="20"/>
+      <c r="K113" s="20"/>
+      <c r="L113" s="38"/>
+      <c r="M113" s="38"/>
+      <c r="N113" s="38"/>
+      <c r="O113" s="27"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P114"/>
     </row>
-    <row r="115" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P115"/>
     </row>
-    <row r="116" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P116"/>
     </row>
-    <row r="117" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P117"/>
     </row>
-    <row r="118" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P118"/>
     </row>
-    <row r="119" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P119"/>
     </row>
-    <row r="120" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P120"/>
     </row>
-    <row r="121" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P121"/>
     </row>
-    <row r="122" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P122"/>
     </row>
-    <row r="123" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P123"/>
     </row>
-    <row r="124" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P124"/>
     </row>
-    <row r="125" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P125"/>
     </row>
-    <row r="126" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P126"/>
     </row>
-    <row r="127" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P127"/>
     </row>
-    <row r="128" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P128"/>
     </row>
     <row r="129" spans="16:16" x14ac:dyDescent="0.4">
@@ -4783,6 +4828,9 @@
     </row>
     <row r="134" spans="16:16" x14ac:dyDescent="0.4">
       <c r="P134"/>
+    </row>
+    <row r="135" spans="16:16" x14ac:dyDescent="0.4">
+      <c r="P135"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4790,15 +4838,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F58" r:id="rId3"/>
+    <hyperlink ref="F59" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
[wk] full respec setting aangepast
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="317">
   <si>
     <t>Name</t>
   </si>
@@ -970,6 +970,12 @@
   </si>
   <si>
     <t>Should an EA toolbox be generated?</t>
+  </si>
+  <si>
+    <t>fullrespec</t>
+  </si>
+  <si>
+    <t>Should a full respec version be generated along with the catalog?</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1120,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1225,6 +1231,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1546,13 +1555,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q135"/>
+  <dimension ref="A1:Q136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomRight" activeCell="O57" sqref="O57:Q57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1743,16 +1752,16 @@
       <c r="P6"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="52" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1767,10 +1776,10 @@
       <c r="P7"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="38"/>
@@ -2853,16 +2862,16 @@
       <c r="P44"/>
     </row>
     <row r="45" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C45" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="51" t="b">
+      <c r="D45" s="52" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
@@ -2880,10 +2889,10 @@
       <c r="P45"/>
     </row>
     <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="51"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
       <c r="G46" s="20"/>
       <c r="K46" s="20"/>
       <c r="L46" s="38"/>
@@ -3155,269 +3164,278 @@
       <c r="O56" s="27"/>
       <c r="P56"/>
     </row>
-    <row r="57" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:16" s="51" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="51" t="s">
+        <v>315</v>
+      </c>
+      <c r="B57" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="27"/>
+      <c r="I57" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="27"/>
+      <c r="M57" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="N57" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" s="27"/>
+      <c r="P57"/>
+    </row>
+    <row r="58" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B58" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C58" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="D57" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="16" t="s">
+      <c r="D58" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G57" s="22"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="16"/>
-      <c r="O57" s="22"/>
-      <c r="P57"/>
-    </row>
-    <row r="58" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
+      <c r="G58" s="22"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="16"/>
+      <c r="O58" s="22"/>
+      <c r="P58"/>
+    </row>
+    <row r="59" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="7" t="s">
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="K58" s="27"/>
-      <c r="O58" s="27"/>
-    </row>
-    <row r="59" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="34" t="s">
-        <v>304</v>
-      </c>
       <c r="G59" s="27"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
       <c r="K59" s="27"/>
       <c r="O59" s="27"/>
     </row>
     <row r="60" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="G60" s="27"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="27"/>
+      <c r="O60" s="27"/>
+    </row>
+    <row r="61" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="O60" s="27"/>
-      <c r="P60"/>
-    </row>
-    <row r="61" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="16" t="s">
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="O61" s="27"/>
+      <c r="P61"/>
+    </row>
+    <row r="62" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B62" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C62" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D61" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="16" t="s">
+      <c r="D62" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="G61" s="22"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="16"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="16"/>
-      <c r="O61" s="22"/>
-      <c r="P61"/>
-    </row>
-    <row r="62" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
+      <c r="G62" s="22"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="22"/>
+      <c r="P62"/>
+    </row>
+    <row r="63" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="7" t="s">
+      <c r="D63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G62" s="20"/>
-      <c r="K62" s="20"/>
-      <c r="O62" s="27"/>
-      <c r="P62"/>
-    </row>
-    <row r="63" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G63" s="20"/>
       <c r="K63" s="20"/>
-      <c r="L63" s="38"/>
-      <c r="M63" s="38"/>
-      <c r="N63" s="38"/>
       <c r="O63" s="27"/>
       <c r="P63"/>
     </row>
-    <row r="64" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D64" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>218</v>
+    <row r="64" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="G64" s="20"/>
       <c r="K64" s="20"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
+      <c r="N64" s="38"/>
       <c r="O64" s="27"/>
       <c r="P64"/>
     </row>
     <row r="65" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>261</v>
-      </c>
-      <c r="B65" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" t="s">
-        <v>262</v>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>226</v>
-      </c>
-      <c r="G65" s="27"/>
-      <c r="K65" s="27"/>
+      <c r="A65" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G65" s="20"/>
+      <c r="K65" s="20"/>
       <c r="O65" s="27"/>
       <c r="P65"/>
     </row>
-    <row r="66" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G66" s="20"/>
-      <c r="K66" s="20"/>
-      <c r="L66" s="38"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="38"/>
+    <row r="66" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>261</v>
+      </c>
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>226</v>
+      </c>
+      <c r="G66" s="27"/>
+      <c r="K66" s="27"/>
       <c r="O66" s="27"/>
       <c r="P66"/>
     </row>
     <row r="67" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
@@ -3426,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>300</v>
+        <v>210</v>
       </c>
       <c r="G67" s="20"/>
       <c r="K67" s="20"/>
@@ -3438,22 +3456,22 @@
     </row>
     <row r="68" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>208</v>
+        <v>300</v>
       </c>
       <c r="G68" s="20"/>
       <c r="K68" s="20"/>
@@ -3463,24 +3481,24 @@
       <c r="O68" s="27"/>
       <c r="P68"/>
     </row>
-    <row r="69" spans="1:17" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="B69" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="D69" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="24" t="s">
-        <v>254</v>
+    <row r="69" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="G69" s="20"/>
       <c r="K69" s="20"/>
@@ -3490,162 +3508,162 @@
       <c r="O69" s="27"/>
       <c r="P69"/>
     </row>
-    <row r="70" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
+    <row r="70" spans="1:17" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D70" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>254</v>
       </c>
       <c r="G70" s="20"/>
-      <c r="H70" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I70" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J70" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K70" s="21"/>
-      <c r="L70" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M70" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N70" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K70" s="20"/>
+      <c r="L70" s="38"/>
+      <c r="M70" s="38"/>
+      <c r="N70" s="38"/>
       <c r="O70" s="27"/>
       <c r="P70"/>
     </row>
     <row r="71" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="B71" s="46" t="s">
+      <c r="A71" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="46" t="s">
-        <v>297</v>
-      </c>
-      <c r="D71" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="46"/>
+      <c r="C71" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="G71" s="20"/>
-      <c r="K71" s="20"/>
-      <c r="L71" s="38"/>
-      <c r="M71" s="38"/>
-      <c r="N71" s="38"/>
+      <c r="H71" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I71" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J71" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K71" s="21"/>
+      <c r="L71" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M71" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N71" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O71" s="27"/>
       <c r="P71"/>
     </row>
-    <row r="72" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D72" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>4</v>
-      </c>
+    <row r="72" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="B72" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="46" t="s">
+        <v>297</v>
+      </c>
+      <c r="D72" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="46"/>
       <c r="G72" s="20"/>
       <c r="K72" s="20"/>
+      <c r="L72" s="38"/>
+      <c r="M72" s="38"/>
+      <c r="N72" s="38"/>
       <c r="O72" s="27"/>
       <c r="P72"/>
     </row>
-    <row r="73" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="40" t="s">
+    <row r="73" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D73" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="O73" s="27"/>
+      <c r="P73"/>
+    </row>
+    <row r="74" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B74" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="40" t="s">
+      <c r="C74" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="D73" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="G73" s="27"/>
-      <c r="L73" s="27"/>
-      <c r="Q73" s="27"/>
-    </row>
-    <row r="74" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" s="20"/>
-      <c r="K74" s="20"/>
-      <c r="L74" s="38"/>
-      <c r="M74" s="38"/>
-      <c r="N74" s="38"/>
-      <c r="O74" s="27"/>
-      <c r="P74"/>
+      <c r="D74" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" s="27"/>
+      <c r="L74" s="27"/>
+      <c r="Q74" s="27"/>
     </row>
     <row r="75" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>77</v>
+        <v>229</v>
       </c>
       <c r="D75" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G75" s="20"/>
       <c r="K75" s="20"/>
@@ -3657,421 +3675,421 @@
     </row>
     <row r="76" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D76" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="33"/>
+      <c r="F76" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G76" s="20"/>
-      <c r="H76" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I76" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J76" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K76" s="21"/>
-      <c r="L76" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M76" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N76" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K76" s="20"/>
+      <c r="L76" s="38"/>
+      <c r="M76" s="38"/>
+      <c r="N76" s="38"/>
       <c r="O76" s="27"/>
       <c r="P76"/>
     </row>
     <row r="77" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D77" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>269</v>
-      </c>
+      <c r="F77" s="33"/>
       <c r="G77" s="20"/>
-      <c r="K77" s="20"/>
-      <c r="L77" s="38"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="38"/>
+      <c r="H77" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I77" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J77" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K77" s="21"/>
+      <c r="L77" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M77" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N77" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O77" s="27"/>
       <c r="P77"/>
     </row>
-    <row r="78" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D78" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>298</v>
+    <row r="78" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="G78" s="20"/>
       <c r="K78" s="20"/>
+      <c r="L78" s="38"/>
+      <c r="M78" s="38"/>
+      <c r="N78" s="38"/>
       <c r="O78" s="27"/>
       <c r="P78"/>
     </row>
-    <row r="79" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>19</v>
+    <row r="79" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>298</v>
       </c>
       <c r="G79" s="20"/>
       <c r="K79" s="20"/>
-      <c r="L79" s="38"/>
-      <c r="M79" s="38"/>
-      <c r="N79" s="38"/>
       <c r="O79" s="27"/>
       <c r="P79"/>
     </row>
-    <row r="80" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A80" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>211</v>
+    <row r="80" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G80" s="20"/>
       <c r="K80" s="20"/>
+      <c r="L80" s="38"/>
+      <c r="M80" s="38"/>
+      <c r="N80" s="38"/>
       <c r="O80" s="27"/>
       <c r="P80"/>
     </row>
-    <row r="81" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
+    <row r="81" spans="1:16" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A81" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D81" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="G81" s="20"/>
-      <c r="H81" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J81" s="17" t="s">
-        <v>278</v>
-      </c>
       <c r="K81" s="20"/>
-      <c r="L81" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="M81" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="N81" s="38" t="s">
-        <v>279</v>
-      </c>
       <c r="O81" s="27"/>
       <c r="P81"/>
     </row>
     <row r="82" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D82" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G82" s="20"/>
+      <c r="H82" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J82" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="K82" s="20"/>
-      <c r="L82" s="38"/>
-      <c r="M82" s="38"/>
-      <c r="N82" s="38"/>
+      <c r="L82" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="M82" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="N82" s="38" t="s">
+        <v>279</v>
+      </c>
       <c r="O82" s="27"/>
       <c r="P82"/>
     </row>
-    <row r="83" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D83" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>92</v>
+    <row r="83" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="G83" s="20"/>
       <c r="K83" s="20"/>
+      <c r="L83" s="38"/>
+      <c r="M83" s="38"/>
+      <c r="N83" s="38"/>
       <c r="O83" s="27"/>
       <c r="P83"/>
     </row>
     <row r="84" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D84" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E84" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="G84" s="20"/>
       <c r="K84" s="20"/>
       <c r="O84" s="27"/>
       <c r="P84"/>
     </row>
-    <row r="85" spans="1:16" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>96</v>
+    <row r="85" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G85" s="20"/>
       <c r="K85" s="20"/>
-      <c r="L85" s="38"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
       <c r="O85" s="27"/>
       <c r="P85"/>
     </row>
-    <row r="86" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:16" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D86" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E86" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G86" s="20"/>
-      <c r="H86" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K86" s="20"/>
-      <c r="L86" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M86" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N86" s="38" t="s">
-        <v>4</v>
-      </c>
+      <c r="L86" s="38"/>
+      <c r="M86" s="38"/>
+      <c r="N86" s="38"/>
       <c r="O86" s="27"/>
       <c r="P86"/>
     </row>
     <row r="87" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
       <c r="D87" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G87" s="20"/>
+      <c r="H87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="K87" s="20"/>
-      <c r="L87" s="38"/>
-      <c r="M87" s="38"/>
-      <c r="N87" s="38"/>
+      <c r="L87" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M87" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N87" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O87" s="27"/>
       <c r="P87"/>
     </row>
-    <row r="88" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B88" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D88" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="G88" s="27"/>
-      <c r="K88" s="27"/>
+    <row r="88" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G88" s="20"/>
+      <c r="K88" s="20"/>
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
       <c r="N88" s="38"/>
       <c r="O88" s="27"/>
       <c r="P88"/>
     </row>
-    <row r="89" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="G89" s="20"/>
-      <c r="K89" s="20"/>
+    <row r="89" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D89" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="G89" s="27"/>
+      <c r="K89" s="27"/>
       <c r="L89" s="38"/>
       <c r="M89" s="38"/>
       <c r="N89" s="38"/>
       <c r="O89" s="27"/>
       <c r="P89"/>
     </row>
-    <row r="90" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="D90" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="6" t="s">
-        <v>250</v>
+    <row r="90" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>251</v>
       </c>
       <c r="G90" s="20"/>
       <c r="K90" s="20"/>
@@ -4081,24 +4099,26 @@
       <c r="O90" s="27"/>
       <c r="P90"/>
     </row>
-    <row r="91" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>298</v>
+    <row r="91" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D91" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="G91" s="20"/>
-      <c r="I91" s="35"/>
-      <c r="J91" s="35"/>
       <c r="K91" s="20"/>
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
@@ -4106,26 +4126,24 @@
       <c r="O91" s="27"/>
       <c r="P91"/>
     </row>
-    <row r="92" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
       <c r="D92" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F92" s="2" t="s">
-        <v>16</v>
+      <c r="F92" s="17" t="s">
+        <v>298</v>
       </c>
       <c r="G92" s="20"/>
+      <c r="I92" s="35"/>
+      <c r="J92" s="35"/>
       <c r="K92" s="20"/>
       <c r="L92" s="38"/>
       <c r="M92" s="38"/>
@@ -4133,65 +4151,65 @@
       <c r="O92" s="27"/>
       <c r="P92"/>
     </row>
-    <row r="93" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
+    <row r="93" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="20"/>
+      <c r="K93" s="20"/>
+      <c r="L93" s="38"/>
+      <c r="M93" s="38"/>
+      <c r="N93" s="38"/>
+      <c r="O93" s="27"/>
+      <c r="P93"/>
+    </row>
+    <row r="94" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
         <v>284</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>10</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>285</v>
       </c>
-      <c r="D93" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="D94" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
         <v>298</v>
       </c>
-      <c r="G93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="O93" s="27"/>
-    </row>
-    <row r="94" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G94" s="20"/>
-      <c r="K94" s="20"/>
-      <c r="L94" s="38"/>
-      <c r="M94" s="38"/>
-      <c r="N94" s="38"/>
+      <c r="G94" s="27"/>
+      <c r="K94" s="27"/>
       <c r="O94" s="27"/>
-      <c r="P94"/>
     </row>
     <row r="95" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
@@ -4199,8 +4217,8 @@
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="2" t="s">
-        <v>16</v>
+      <c r="F95" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="G95" s="20"/>
       <c r="K95" s="20"/>
@@ -4210,21 +4228,24 @@
       <c r="O95" s="27"/>
       <c r="P95"/>
     </row>
-    <row r="96" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D96" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G96" s="20"/>
       <c r="K96" s="20"/>
@@ -4236,22 +4257,19 @@
     </row>
     <row r="97" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D97" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="G97" s="20"/>
       <c r="K97" s="20"/>
@@ -4261,15 +4279,15 @@
       <c r="O97" s="27"/>
       <c r="P97"/>
     </row>
-    <row r="98" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>1</v>
@@ -4277,62 +4295,65 @@
       <c r="E98" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F98" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G98" s="20"/>
-      <c r="H98" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I98" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J98" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K98" s="21"/>
-      <c r="L98" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M98" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N98" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K98" s="20"/>
+      <c r="L98" s="38"/>
+      <c r="M98" s="38"/>
+      <c r="N98" s="38"/>
       <c r="O98" s="27"/>
       <c r="P98"/>
     </row>
-    <row r="99" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D99" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>218</v>
+    <row r="99" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G99" s="20"/>
-      <c r="K99" s="20"/>
+      <c r="H99" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I99" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J99" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K99" s="21"/>
+      <c r="L99" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M99" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N99" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O99" s="27"/>
       <c r="P99"/>
     </row>
     <row r="100" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D100" s="7" t="b">
         <v>1</v>
@@ -4350,79 +4371,64 @@
     </row>
     <row r="101" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D101" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E101" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="G101" s="20"/>
       <c r="K101" s="20"/>
       <c r="O101" s="27"/>
       <c r="P101"/>
     </row>
-    <row r="102" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B102" s="2" t="s">
+    <row r="102" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>1</v>
+      <c r="C102" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D102" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G102" s="20"/>
-      <c r="H102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K102" s="20"/>
-      <c r="L102" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="M102" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N102" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="O102" s="27"/>
       <c r="P102"/>
     </row>
     <row r="103" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D103" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
@@ -4452,23 +4458,23 @@
     </row>
     <row r="104" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D104" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G104" s="20"/>
       <c r="H104" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>4</v>
@@ -4478,7 +4484,7 @@
       </c>
       <c r="K104" s="20"/>
       <c r="L104" s="38" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="M104" s="38" t="s">
         <v>4</v>
@@ -4489,15 +4495,15 @@
       <c r="O104" s="27"/>
       <c r="P104"/>
     </row>
-    <row r="105" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="D105" s="2" t="b">
         <v>0</v>
@@ -4505,119 +4511,120 @@
       <c r="E105" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F105" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G105" s="20"/>
-      <c r="H105"/>
-      <c r="I105"/>
-      <c r="J105"/>
+      <c r="H105" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="K105" s="20"/>
-      <c r="L105" s="38"/>
-      <c r="M105" s="38"/>
-      <c r="N105" s="38"/>
+      <c r="L105" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M105" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N105" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O105" s="27"/>
       <c r="P105"/>
     </row>
-    <row r="106" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" t="s">
-        <v>286</v>
-      </c>
-      <c r="B106" t="s">
+    <row r="106" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C106" t="s">
-        <v>287</v>
-      </c>
-      <c r="D106" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" t="s">
-        <v>4</v>
-      </c>
-      <c r="G106" s="27"/>
+      <c r="C106" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="20"/>
       <c r="H106"/>
       <c r="I106"/>
       <c r="J106"/>
-      <c r="K106" s="27"/>
-      <c r="L106"/>
-      <c r="M106"/>
-      <c r="N106"/>
+      <c r="K106" s="20"/>
+      <c r="L106" s="38"/>
+      <c r="M106" s="38"/>
+      <c r="N106" s="38"/>
       <c r="O106" s="27"/>
-    </row>
-    <row r="107" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A107" s="7" t="s">
+      <c r="P106"/>
+    </row>
+    <row r="107" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
+        <v>286</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>287</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" t="s">
+        <v>4</v>
+      </c>
+      <c r="G107" s="27"/>
+      <c r="H107"/>
+      <c r="I107"/>
+      <c r="J107"/>
+      <c r="K107" s="27"/>
+      <c r="L107"/>
+      <c r="M107"/>
+      <c r="N107"/>
+      <c r="O107" s="27"/>
+    </row>
+    <row r="108" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B108" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C108" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D107" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G107" s="20"/>
-      <c r="K107" s="20"/>
-      <c r="O107" s="27"/>
-    </row>
-    <row r="108" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="b">
-        <v>1</v>
+      <c r="D108" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G108" s="20"/>
-      <c r="H108" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K108" s="20"/>
-      <c r="L108" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M108" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N108" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="O108" s="27"/>
     </row>
     <row r="109" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D109" s="2" t="b">
         <v>1</v>
@@ -4649,125 +4656,160 @@
     </row>
     <row r="110" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G110" s="20"/>
+      <c r="H110" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K110" s="20"/>
+      <c r="L110" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M110" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N110" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="O110" s="27"/>
+    </row>
+    <row r="111" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F110" s="47" t="s">
+      <c r="D111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" s="47" t="s">
         <v>298</v>
       </c>
-      <c r="G110" s="20"/>
-      <c r="K110" s="20"/>
-      <c r="L110" s="38"/>
-      <c r="M110" s="38"/>
-      <c r="N110" s="38"/>
-      <c r="O110" s="27"/>
-    </row>
-    <row r="111" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="48" t="s">
+      <c r="G111" s="20"/>
+      <c r="K111" s="20"/>
+      <c r="L111" s="38"/>
+      <c r="M111" s="38"/>
+      <c r="N111" s="38"/>
+      <c r="O111" s="27"/>
+    </row>
+    <row r="112" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="B111" s="48" t="s">
+      <c r="B112" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C111" s="48" t="s">
+      <c r="C112" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="D111" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="G111" s="27"/>
-      <c r="H111" s="48" t="s">
+      <c r="D112" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" s="27"/>
+      <c r="H112" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="I111" s="48" t="s">
+      <c r="I112" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="J111" s="48" t="s">
+      <c r="J112" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="K111" s="21"/>
-      <c r="L111" s="48" t="s">
+      <c r="K112" s="21"/>
+      <c r="L112" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="M111" s="48" t="s">
+      <c r="M112" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="N111" s="48" t="s">
+      <c r="N112" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="O111" s="27"/>
-    </row>
-    <row r="112" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A112" s="26" t="s">
+      <c r="O112" s="27"/>
+    </row>
+    <row r="113" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A113" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B112" s="26" t="s">
+      <c r="B113" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C112" s="26" t="s">
+      <c r="C113" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="D112" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="26" t="s">
+      <c r="D113" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="G112" s="27"/>
-      <c r="H112" s="26"/>
-      <c r="I112" s="26"/>
-      <c r="J112" s="26"/>
-      <c r="K112" s="27"/>
-      <c r="L112" s="38"/>
-      <c r="M112" s="38"/>
-      <c r="N112" s="38"/>
-      <c r="O112" s="27"/>
-    </row>
-    <row r="113" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A113" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G113" s="20"/>
-      <c r="K113" s="20"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="27"/>
       <c r="L113" s="38"/>
       <c r="M113" s="38"/>
       <c r="N113" s="38"/>
       <c r="O113" s="27"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P114"/>
+    <row r="114" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A114" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G114" s="20"/>
+      <c r="K114" s="20"/>
+      <c r="L114" s="38"/>
+      <c r="M114" s="38"/>
+      <c r="N114" s="38"/>
+      <c r="O114" s="27"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P115"/>
@@ -4831,6 +4873,9 @@
     </row>
     <row r="135" spans="16:16" x14ac:dyDescent="0.4">
       <c r="P135"/>
+    </row>
+    <row r="136" spans="16:16" x14ac:dyDescent="0.4">
+      <c r="P136"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4846,7 +4891,7 @@
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F59" r:id="rId3"/>
+    <hyperlink ref="F60" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
[wk] dead links check, cli/signaldeadurls toegevoegd
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="323">
   <si>
     <t>Name</t>
   </si>
@@ -988,6 +988,12 @@
   </si>
   <si>
     <t>Yes if MIM format must be generated</t>
+  </si>
+  <si>
+    <t>signaldeadurls</t>
+  </si>
+  <si>
+    <t>Yes if a warning should, be issued for each inaccessible URL detected in notes and tagged values.</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1138,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1243,6 +1249,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1570,13 +1579,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q138"/>
+  <dimension ref="A1:Q139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N38" sqref="N38"/>
+      <selection pane="bottomRight" activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1767,16 +1776,16 @@
       <c r="P6"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53" t="b">
+      <c r="D7" s="54" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1791,10 +1800,10 @@
       <c r="P7"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
       <c r="G8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="38"/>
@@ -2900,16 +2909,16 @@
       <c r="P45"/>
     </row>
     <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="53" t="s">
+      <c r="A46" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="53" t="s">
+      <c r="C46" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="53" t="b">
+      <c r="D46" s="54" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -2927,10 +2936,10 @@
       <c r="P46"/>
     </row>
     <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="53"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
+      <c r="A47" s="54"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
       <c r="G47" s="20"/>
       <c r="K47" s="20"/>
       <c r="L47" s="38"/>
@@ -4161,51 +4170,56 @@
       <c r="O92" s="27"/>
       <c r="P92"/>
     </row>
-    <row r="93" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="D93" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="G93" s="20"/>
-      <c r="K93" s="20"/>
-      <c r="L93" s="38"/>
-      <c r="M93" s="38"/>
-      <c r="N93" s="38"/>
+    <row r="93" spans="1:16" s="53" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="53" t="s">
+        <v>321</v>
+      </c>
+      <c r="B93" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="53" t="s">
+        <v>322</v>
+      </c>
+      <c r="D93" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="27"/>
+      <c r="I93" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="J93" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="K93" s="27"/>
       <c r="O93" s="27"/>
       <c r="P93"/>
     </row>
-    <row r="94" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="17" t="s">
-        <v>298</v>
+    <row r="94" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D94" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="G94" s="20"/>
-      <c r="I94" s="35"/>
-      <c r="J94" s="35"/>
       <c r="K94" s="20"/>
       <c r="L94" s="38"/>
       <c r="M94" s="38"/>
@@ -4213,26 +4227,24 @@
       <c r="O94" s="27"/>
       <c r="P94"/>
     </row>
-    <row r="95" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
       <c r="D95" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="2" t="s">
-        <v>16</v>
+      <c r="F95" s="17" t="s">
+        <v>298</v>
       </c>
       <c r="G95" s="20"/>
+      <c r="I95" s="35"/>
+      <c r="J95" s="35"/>
       <c r="K95" s="20"/>
       <c r="L95" s="38"/>
       <c r="M95" s="38"/>
@@ -4240,65 +4252,65 @@
       <c r="O95" s="27"/>
       <c r="P95"/>
     </row>
-    <row r="96" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A96" t="s">
+    <row r="96" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="38"/>
+      <c r="M96" s="38"/>
+      <c r="N96" s="38"/>
+      <c r="O96" s="27"/>
+      <c r="P96"/>
+    </row>
+    <row r="97" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
         <v>284</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>10</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>285</v>
       </c>
-      <c r="D96" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="D97" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
         <v>298</v>
       </c>
-      <c r="G96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="O96" s="27"/>
-    </row>
-    <row r="97" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G97" s="20"/>
-      <c r="K97" s="20"/>
-      <c r="L97" s="38"/>
-      <c r="M97" s="38"/>
-      <c r="N97" s="38"/>
+      <c r="G97" s="27"/>
+      <c r="K97" s="27"/>
       <c r="O97" s="27"/>
-      <c r="P97"/>
     </row>
     <row r="98" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
@@ -4306,8 +4318,8 @@
       <c r="E98" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F98" s="2" t="s">
-        <v>16</v>
+      <c r="F98" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="G98" s="20"/>
       <c r="K98" s="20"/>
@@ -4317,21 +4329,24 @@
       <c r="O98" s="27"/>
       <c r="P98"/>
     </row>
-    <row r="99" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E99" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G99" s="20"/>
       <c r="K99" s="20"/>
@@ -4343,22 +4358,19 @@
     </row>
     <row r="100" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D100" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="G100" s="20"/>
       <c r="K100" s="20"/>
@@ -4368,15 +4380,15 @@
       <c r="O100" s="27"/>
       <c r="P100"/>
     </row>
-    <row r="101" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>1</v>
@@ -4384,62 +4396,65 @@
       <c r="E101" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F101" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G101" s="20"/>
-      <c r="H101" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="I101" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="J101" s="47" t="s">
-        <v>302</v>
-      </c>
-      <c r="K101" s="21"/>
-      <c r="L101" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M101" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N101" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="K101" s="20"/>
+      <c r="L101" s="38"/>
+      <c r="M101" s="38"/>
+      <c r="N101" s="38"/>
       <c r="O101" s="27"/>
       <c r="P101"/>
     </row>
-    <row r="102" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D102" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>218</v>
+    <row r="102" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G102" s="20"/>
-      <c r="K102" s="20"/>
+      <c r="H102" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="I102" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="J102" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="K102" s="21"/>
+      <c r="L102" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="M102" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="N102" s="47" t="s">
+        <v>301</v>
+      </c>
       <c r="O102" s="27"/>
       <c r="P102"/>
     </row>
     <row r="103" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D103" s="7" t="b">
         <v>1</v>
@@ -4457,79 +4472,64 @@
     </row>
     <row r="104" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D104" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E104" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="G104" s="20"/>
       <c r="K104" s="20"/>
       <c r="O104" s="27"/>
       <c r="P104"/>
     </row>
-    <row r="105" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="2" t="s">
+    <row r="105" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D105" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" s="2" t="b">
-        <v>1</v>
+      <c r="C105" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G105" s="20"/>
-      <c r="H105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J105" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K105" s="20"/>
-      <c r="L105" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="M105" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N105" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="O105" s="27"/>
       <c r="P105"/>
     </row>
     <row r="106" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D106" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="2" t="b">
         <v>1</v>
@@ -4559,23 +4559,23 @@
     </row>
     <row r="107" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D107" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G107" s="20"/>
       <c r="H107" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>4</v>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="K107" s="20"/>
       <c r="L107" s="38" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="M107" s="38" t="s">
         <v>4</v>
@@ -4596,15 +4596,15 @@
       <c r="O107" s="27"/>
       <c r="P107"/>
     </row>
-    <row r="108" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>0</v>
@@ -4612,119 +4612,120 @@
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G108" s="20"/>
-      <c r="H108"/>
-      <c r="I108"/>
-      <c r="J108"/>
+      <c r="H108" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="K108" s="20"/>
-      <c r="L108" s="38"/>
-      <c r="M108" s="38"/>
-      <c r="N108" s="38"/>
+      <c r="L108" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M108" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N108" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="O108" s="27"/>
       <c r="P108"/>
     </row>
-    <row r="109" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>286</v>
-      </c>
-      <c r="B109" t="s">
+    <row r="109" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A109" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C109" t="s">
-        <v>287</v>
-      </c>
-      <c r="D109" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
-        <v>4</v>
-      </c>
-      <c r="G109" s="27"/>
+      <c r="C109" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="20"/>
       <c r="H109"/>
       <c r="I109"/>
       <c r="J109"/>
-      <c r="K109" s="27"/>
-      <c r="L109"/>
-      <c r="M109"/>
-      <c r="N109"/>
+      <c r="K109" s="20"/>
+      <c r="L109" s="38"/>
+      <c r="M109" s="38"/>
+      <c r="N109" s="38"/>
       <c r="O109" s="27"/>
-    </row>
-    <row r="110" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A110" s="7" t="s">
+      <c r="P109"/>
+    </row>
+    <row r="110" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
+        <v>286</v>
+      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>287</v>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" t="s">
+        <v>4</v>
+      </c>
+      <c r="G110" s="27"/>
+      <c r="H110"/>
+      <c r="I110"/>
+      <c r="J110"/>
+      <c r="K110" s="27"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110" s="27"/>
+    </row>
+    <row r="111" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A111" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B110" s="7" t="s">
+      <c r="B111" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C111" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D110" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F110" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G110" s="20"/>
-      <c r="K110" s="20"/>
-      <c r="O110" s="27"/>
-    </row>
-    <row r="111" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>1</v>
+      <c r="D111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G111" s="20"/>
-      <c r="H111" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="K111" s="20"/>
-      <c r="L111" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M111" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N111" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="O111" s="27"/>
     </row>
     <row r="112" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D112" s="2" t="b">
         <v>1</v>
@@ -4756,125 +4757,160 @@
     </row>
     <row r="113" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" s="20"/>
+      <c r="H113" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K113" s="20"/>
+      <c r="L113" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="O113" s="27"/>
+    </row>
+    <row r="114" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F113" s="47" t="s">
+      <c r="D114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" s="47" t="s">
         <v>298</v>
       </c>
-      <c r="G113" s="20"/>
-      <c r="K113" s="20"/>
-      <c r="L113" s="38"/>
-      <c r="M113" s="38"/>
-      <c r="N113" s="38"/>
-      <c r="O113" s="27"/>
-    </row>
-    <row r="114" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="48" t="s">
+      <c r="G114" s="20"/>
+      <c r="K114" s="20"/>
+      <c r="L114" s="38"/>
+      <c r="M114" s="38"/>
+      <c r="N114" s="38"/>
+      <c r="O114" s="27"/>
+    </row>
+    <row r="115" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="B114" s="48" t="s">
+      <c r="B115" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="48" t="s">
+      <c r="C115" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="D114" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="G114" s="27"/>
-      <c r="H114" s="48" t="s">
+      <c r="D115" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" s="27"/>
+      <c r="H115" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="I114" s="48" t="s">
+      <c r="I115" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="J114" s="48" t="s">
+      <c r="J115" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="K114" s="21"/>
-      <c r="L114" s="48" t="s">
+      <c r="K115" s="21"/>
+      <c r="L115" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="M114" s="48" t="s">
+      <c r="M115" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="N114" s="48" t="s">
+      <c r="N115" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="O114" s="27"/>
-    </row>
-    <row r="115" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A115" s="26" t="s">
+      <c r="O115" s="27"/>
+    </row>
+    <row r="116" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A116" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B115" s="26" t="s">
+      <c r="B116" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C115" s="26" t="s">
+      <c r="C116" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="D115" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" s="26" t="s">
+      <c r="D116" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="G115" s="27"/>
-      <c r="H115" s="26"/>
-      <c r="I115" s="26"/>
-      <c r="J115" s="26"/>
-      <c r="K115" s="27"/>
-      <c r="L115" s="38"/>
-      <c r="M115" s="38"/>
-      <c r="N115" s="38"/>
-      <c r="O115" s="27"/>
-    </row>
-    <row r="116" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A116" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D116" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G116" s="20"/>
-      <c r="K116" s="20"/>
+      <c r="G116" s="27"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="26"/>
+      <c r="K116" s="27"/>
       <c r="L116" s="38"/>
       <c r="M116" s="38"/>
       <c r="N116" s="38"/>
       <c r="O116" s="27"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P117"/>
+    <row r="117" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A117" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G117" s="20"/>
+      <c r="K117" s="20"/>
+      <c r="L117" s="38"/>
+      <c r="M117" s="38"/>
+      <c r="N117" s="38"/>
+      <c r="O117" s="27"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.4">
       <c r="P118"/>
@@ -4938,6 +4974,9 @@
     </row>
     <row r="138" spans="16:16" x14ac:dyDescent="0.4">
       <c r="P138"/>
+    </row>
+    <row r="139" spans="16:16" x14ac:dyDescent="0.4">
+      <c r="P139"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[WK] Waarderingskamer volgt UGM van VNGR
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="329">
   <si>
     <t>Name</t>
   </si>
@@ -994,6 +994,24 @@
   </si>
   <si>
     <t>Yes if a warning should, be issued for each inaccessible URL detected in notes and tagged values.</t>
+  </si>
+  <si>
+    <t>UGM: minimum</t>
+  </si>
+  <si>
+    <t>UGM: uitgebreid</t>
+  </si>
+  <si>
+    <t>UGM: opleveren</t>
+  </si>
+  <si>
+    <t>UGM</t>
+  </si>
+  <si>
+    <t>WaarderingskamerUGM</t>
+  </si>
+  <si>
+    <t>WKUGM</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1156,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1249,6 +1267,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1579,13 +1600,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q139"/>
+  <dimension ref="A1:T139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C97" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K93" sqref="K93"/>
+      <selection pane="bottomRight" activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1600,14 +1621,18 @@
     <col min="8" max="9" width="14.765625" customWidth="1"/>
     <col min="10" max="10" width="14.3046875" customWidth="1"/>
     <col min="11" max="11" width="5.4609375" style="23" customWidth="1"/>
-    <col min="12" max="12" width="16.15234375" customWidth="1"/>
-    <col min="13" max="13" width="16.07421875" customWidth="1"/>
-    <col min="14" max="14" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.3046875" customWidth="1"/>
+    <col min="13" max="13" width="25.3828125" customWidth="1"/>
+    <col min="14" max="14" width="26.921875" customWidth="1"/>
     <col min="15" max="15" width="5.4609375" style="23" customWidth="1"/>
-    <col min="16" max="16" width="27.3046875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.15234375" customWidth="1"/>
+    <col min="17" max="17" width="16.07421875" customWidth="1"/>
+    <col min="18" max="18" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.4609375" style="23" customWidth="1"/>
+    <col min="20" max="20" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1647,11 +1672,21 @@
         <v>252</v>
       </c>
       <c r="O1" s="18"/>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="S1" s="18"/>
+      <c r="T1" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="19"/>
       <c r="H2" s="3" t="s">
@@ -1665,18 +1700,28 @@
       </c>
       <c r="K2" s="19"/>
       <c r="L2" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="O2" s="19"/>
+      <c r="P2" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="S2" s="19"/>
+      <c r="T2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -1694,13 +1739,17 @@
       </c>
       <c r="G3" s="20"/>
       <c r="K3" s="20"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
       <c r="O3" s="27"/>
-      <c r="P3"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="27"/>
+      <c r="T3"/>
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1721,13 +1770,17 @@
       </c>
       <c r="G4" s="20"/>
       <c r="K4" s="20"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
       <c r="O4" s="27"/>
-      <c r="P4"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="27"/>
+      <c r="T4"/>
+    </row>
+    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1748,13 +1801,17 @@
       </c>
       <c r="G5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
       <c r="O5" s="27"/>
-      <c r="P5"/>
-    </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="27"/>
+      <c r="T5"/>
+    </row>
+    <row r="6" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>157</v>
       </c>
@@ -1773,19 +1830,20 @@
       <c r="G6" s="20"/>
       <c r="K6" s="20"/>
       <c r="O6" s="27"/>
-      <c r="P6"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="54" t="s">
+      <c r="S6" s="27"/>
+      <c r="T6"/>
+    </row>
+    <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="54" t="b">
+      <c r="D7" s="55" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1793,26 +1851,34 @@
       </c>
       <c r="G7" s="20"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
       <c r="O7" s="27"/>
-      <c r="P7"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="54"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="27"/>
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
       <c r="G8" s="20"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
       <c r="O8" s="27"/>
-      <c r="P8"/>
-    </row>
-    <row r="9" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="27"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>160</v>
       </c>
@@ -1834,9 +1900,10 @@
       <c r="G9" s="20"/>
       <c r="K9" s="20"/>
       <c r="O9" s="27"/>
-      <c r="P9"/>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S9" s="27"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1857,13 +1924,17 @@
       </c>
       <c r="G10" s="20"/>
       <c r="K10" s="20"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
       <c r="O10" s="27"/>
-      <c r="P10"/>
-    </row>
-    <row r="11" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="27"/>
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>162</v>
       </c>
@@ -1882,9 +1953,10 @@
       <c r="G11" s="20"/>
       <c r="K11" s="20"/>
       <c r="O11" s="27"/>
-      <c r="P11"/>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S11" s="27"/>
+      <c r="T11"/>
+    </row>
+    <row r="12" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>135</v>
       </c>
@@ -1905,13 +1977,17 @@
       </c>
       <c r="G12" s="20"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
       <c r="O12" s="27"/>
-      <c r="P12"/>
-    </row>
-    <row r="13" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="27"/>
+      <c r="T12"/>
+    </row>
+    <row r="13" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
         <v>243</v>
       </c>
@@ -1932,13 +2008,17 @@
       </c>
       <c r="G13" s="20"/>
       <c r="K13" s="20"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
       <c r="O13" s="27"/>
-      <c r="P13"/>
-    </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="27"/>
+      <c r="T13"/>
+    </row>
+    <row r="14" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1959,13 +2039,17 @@
       </c>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
       <c r="O14" s="27"/>
-      <c r="P14"/>
-    </row>
-    <row r="15" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="27"/>
+      <c r="T14"/>
+    </row>
+    <row r="15" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1992,19 +2076,29 @@
         <v>205</v>
       </c>
       <c r="K15" s="20"/>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="38" t="s">
+      <c r="N15" s="54" t="s">
         <v>205</v>
       </c>
       <c r="O15" s="27"/>
-      <c r="P15"/>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P15" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="R15" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="S15" s="27"/>
+      <c r="T15"/>
+    </row>
+    <row r="16" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2025,13 +2119,17 @@
       </c>
       <c r="G16" s="20"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
       <c r="O16" s="27"/>
-      <c r="P16"/>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="27"/>
+      <c r="T16"/>
+    </row>
+    <row r="17" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>221</v>
       </c>
@@ -2052,13 +2150,17 @@
       </c>
       <c r="G17" s="20"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
       <c r="O17" s="27"/>
-      <c r="P17"/>
-    </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="27"/>
+      <c r="T17"/>
+    </row>
+    <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>223</v>
       </c>
@@ -2075,13 +2177,17 @@
       </c>
       <c r="G18" s="20"/>
       <c r="K18" s="20"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
       <c r="O18" s="27"/>
-      <c r="P18"/>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="27"/>
+      <c r="T18"/>
+    </row>
+    <row r="19" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -2099,13 +2205,17 @@
       </c>
       <c r="G19" s="20"/>
       <c r="K19" s="20"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
       <c r="O19" s="27"/>
-      <c r="P19"/>
-    </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="27"/>
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>137</v>
       </c>
@@ -2126,13 +2236,17 @@
       </c>
       <c r="G20" s="20"/>
       <c r="K20" s="20"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
       <c r="O20" s="27"/>
-      <c r="P20"/>
-    </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="27"/>
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>140</v>
       </c>
@@ -2153,13 +2267,17 @@
       </c>
       <c r="G21" s="20"/>
       <c r="K21" s="20"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
       <c r="O21" s="27"/>
-      <c r="P21"/>
-    </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="27"/>
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>143</v>
       </c>
@@ -2186,19 +2304,29 @@
         <v>4</v>
       </c>
       <c r="K22" s="20"/>
-      <c r="L22" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N22" s="38" t="s">
+      <c r="L22" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O22" s="27"/>
-      <c r="P22"/>
-    </row>
-    <row r="23" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P22" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R22" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S22" s="27"/>
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2220,9 +2348,10 @@
       <c r="G23" s="20"/>
       <c r="K23" s="20"/>
       <c r="O23" s="27"/>
-      <c r="P23"/>
-    </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S23" s="27"/>
+      <c r="T23"/>
+    </row>
+    <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>166</v>
       </c>
@@ -2240,13 +2369,17 @@
       </c>
       <c r="G24" s="20"/>
       <c r="K24" s="20"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
       <c r="O24" s="27"/>
-      <c r="P24"/>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="27"/>
+      <c r="T24"/>
+    </row>
+    <row r="25" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2273,19 +2406,29 @@
         <v>4</v>
       </c>
       <c r="K25" s="20"/>
-      <c r="L25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25" s="38" t="s">
+      <c r="L25" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O25" s="27"/>
-      <c r="P25"/>
-    </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P25" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q25" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="R25" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S25" s="27"/>
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2312,19 +2455,29 @@
         <v>4</v>
       </c>
       <c r="K26" s="20"/>
-      <c r="L26" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" s="38" t="s">
+      <c r="L26" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O26" s="27"/>
-      <c r="P26"/>
-    </row>
-    <row r="27" spans="1:16" s="50" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P26" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q26" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R26" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="27"/>
+      <c r="T26"/>
+    </row>
+    <row r="27" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="50" t="s">
         <v>313</v>
       </c>
@@ -2351,19 +2504,29 @@
         <v>4</v>
       </c>
       <c r="K27" s="27"/>
-      <c r="L27" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" s="50" t="s">
+      <c r="L27" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N27" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O27" s="27"/>
-      <c r="P27"/>
-    </row>
-    <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P27" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="R27" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="S27" s="27"/>
+      <c r="T27"/>
+    </row>
+    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2390,19 +2553,29 @@
         <v>4</v>
       </c>
       <c r="K28" s="20"/>
-      <c r="L28" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" s="38" t="s">
+      <c r="L28" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O28" s="27"/>
-      <c r="P28"/>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="R28" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S28" s="27"/>
+      <c r="T28"/>
+    </row>
+    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>145</v>
       </c>
@@ -2429,19 +2602,29 @@
         <v>4</v>
       </c>
       <c r="K29" s="20"/>
-      <c r="L29" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M29" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N29" s="38" t="s">
+      <c r="L29" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O29" s="27"/>
-      <c r="P29"/>
-    </row>
-    <row r="30" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q29" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R29" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S29" s="27"/>
+      <c r="T29"/>
+    </row>
+    <row r="30" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="28" t="s">
         <v>259</v>
       </c>
@@ -2464,13 +2647,17 @@
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
       <c r="K30" s="27"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
       <c r="O30" s="27"/>
-      <c r="P30"/>
-    </row>
-    <row r="31" spans="1:16" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P30" s="43"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="27"/>
+      <c r="T30"/>
+    </row>
+    <row r="31" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="30" t="s">
         <v>264</v>
       </c>
@@ -2494,19 +2681,17 @@
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
       <c r="K31" s="27"/>
-      <c r="L31" s="38" t="s">
-        <v>301</v>
-      </c>
-      <c r="M31" s="45" t="s">
-        <v>301</v>
-      </c>
-      <c r="N31" s="45" t="s">
-        <v>301</v>
-      </c>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
       <c r="O31" s="27"/>
-      <c r="P31"/>
-    </row>
-    <row r="32" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P31" s="38"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="27"/>
+      <c r="T31"/>
+    </row>
+    <row r="32" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2533,19 +2718,29 @@
         <v>34</v>
       </c>
       <c r="K32" s="20"/>
-      <c r="L32" s="42" t="s">
+      <c r="L32" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="M32" s="42" t="s">
+      <c r="M32" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="N32" s="42" t="s">
+      <c r="N32" s="54" t="s">
         <v>19</v>
       </c>
       <c r="O32" s="27"/>
-      <c r="P32"/>
-    </row>
-    <row r="33" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P32" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="R32" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="S32" s="27"/>
+      <c r="T32"/>
+    </row>
+    <row r="33" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>168</v>
       </c>
@@ -2566,13 +2761,17 @@
       </c>
       <c r="G33" s="20"/>
       <c r="K33" s="20"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
       <c r="O33" s="27"/>
-      <c r="P33"/>
-    </row>
-    <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="27"/>
+      <c r="T33"/>
+    </row>
+    <row r="34" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>171</v>
       </c>
@@ -2593,13 +2792,17 @@
       </c>
       <c r="G34" s="20"/>
       <c r="K34" s="20"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="54"/>
+      <c r="N34" s="54"/>
       <c r="O34" s="27"/>
-      <c r="P34"/>
-    </row>
-    <row r="35" spans="1:16" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="27"/>
+      <c r="T34"/>
+    </row>
+    <row r="35" spans="1:20" s="37" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="37" t="s">
         <v>270</v>
       </c>
@@ -2620,12 +2823,16 @@
       </c>
       <c r="G35" s="27"/>
       <c r="K35" s="27"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="54"/>
+      <c r="N35" s="54"/>
       <c r="O35" s="27"/>
-    </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="27"/>
+    </row>
+    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -2646,13 +2853,17 @@
       </c>
       <c r="G36" s="20"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54"/>
       <c r="O36" s="27"/>
-      <c r="P36"/>
-    </row>
-    <row r="37" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P36" s="38"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="27"/>
+      <c r="T36"/>
+    </row>
+    <row r="37" spans="1:20" s="40" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="40" t="s">
         <v>282</v>
       </c>
@@ -2674,8 +2885,9 @@
       <c r="G37" s="41"/>
       <c r="K37" s="41"/>
       <c r="O37" s="41"/>
-    </row>
-    <row r="38" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S37" s="41"/>
+    </row>
+    <row r="38" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="52" t="s">
         <v>319</v>
       </c>
@@ -2696,9 +2908,13 @@
       </c>
       <c r="G38" s="27"/>
       <c r="K38" s="27"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
       <c r="O38" s="27"/>
-    </row>
-    <row r="39" spans="1:16" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="S38" s="27"/>
+    </row>
+    <row r="39" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -2719,13 +2935,17 @@
       </c>
       <c r="G39" s="20"/>
       <c r="K39" s="20"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
-      <c r="N39" s="38"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="54"/>
+      <c r="N39" s="54"/>
       <c r="O39" s="27"/>
-      <c r="P39"/>
-    </row>
-    <row r="40" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
+      <c r="S39" s="27"/>
+      <c r="T39"/>
+    </row>
+    <row r="40" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -2746,13 +2966,17 @@
       </c>
       <c r="G40" s="20"/>
       <c r="K40" s="20"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
+      <c r="L40" s="54"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="54"/>
       <c r="O40" s="27"/>
-      <c r="P40"/>
-    </row>
-    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="27"/>
+      <c r="T40"/>
+    </row>
+    <row r="41" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -2773,13 +2997,17 @@
       </c>
       <c r="G41" s="20"/>
       <c r="K41" s="20"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="54"/>
+      <c r="N41" s="54"/>
       <c r="O41" s="27"/>
-      <c r="P41"/>
-    </row>
-    <row r="42" spans="1:16" s="30" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+      <c r="S41" s="27"/>
+      <c r="T41"/>
+    </row>
+    <row r="42" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="30" t="s">
         <v>263</v>
       </c>
@@ -2799,29 +3027,21 @@
         <v>296</v>
       </c>
       <c r="G42" s="27"/>
-      <c r="H42" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="I42" s="39" t="s">
-        <v>302</v>
-      </c>
-      <c r="J42" s="39" t="s">
-        <v>302</v>
-      </c>
+      <c r="H42" s="36"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
       <c r="K42" s="27"/>
-      <c r="L42" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="M42" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="N42" s="47" t="s">
-        <v>301</v>
-      </c>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54"/>
       <c r="O42" s="27"/>
-      <c r="P42"/>
-    </row>
-    <row r="43" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="27"/>
+      <c r="T42"/>
+    </row>
+    <row r="43" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>174</v>
       </c>
@@ -2848,19 +3068,29 @@
         <v>16</v>
       </c>
       <c r="K43" s="20"/>
-      <c r="L43" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="M43" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N43" s="38" t="s">
+      <c r="L43" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N43" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O43" s="27"/>
-      <c r="P43"/>
-    </row>
-    <row r="44" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P43" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q43" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R43" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S43" s="27"/>
+      <c r="T43"/>
+    </row>
+    <row r="44" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
@@ -2882,9 +3112,10 @@
       <c r="G44" s="20"/>
       <c r="K44" s="20"/>
       <c r="O44" s="27"/>
-      <c r="P44"/>
-    </row>
-    <row r="45" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S44" s="27"/>
+      <c r="T44"/>
+    </row>
+    <row r="45" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>47</v>
       </c>
@@ -2906,19 +3137,20 @@
       <c r="G45" s="20"/>
       <c r="K45" s="20"/>
       <c r="O45" s="27"/>
-      <c r="P45"/>
-    </row>
-    <row r="46" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="54" t="s">
+      <c r="S45" s="27"/>
+      <c r="T45"/>
+    </row>
+    <row r="46" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="54" t="s">
+      <c r="C46" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="54" t="b">
+      <c r="D46" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -2929,26 +3161,34 @@
       </c>
       <c r="G46" s="20"/>
       <c r="K46" s="20"/>
-      <c r="L46" s="38"/>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
+      <c r="L46" s="54"/>
+      <c r="M46" s="54"/>
+      <c r="N46" s="54"/>
       <c r="O46" s="27"/>
-      <c r="P46"/>
-    </row>
-    <row r="47" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="54"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="38"/>
+      <c r="R46" s="38"/>
+      <c r="S46" s="27"/>
+      <c r="T46"/>
+    </row>
+    <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="55"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
       <c r="G47" s="20"/>
       <c r="K47" s="20"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38"/>
-      <c r="N47" s="38"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="54"/>
+      <c r="N47" s="54"/>
       <c r="O47" s="27"/>
-      <c r="P47"/>
-    </row>
-    <row r="48" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P47" s="38"/>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="38"/>
+      <c r="S47" s="27"/>
+      <c r="T47"/>
+    </row>
+    <row r="48" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>176</v>
       </c>
@@ -2966,13 +3206,17 @@
       </c>
       <c r="G48" s="20"/>
       <c r="K48" s="20"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="38"/>
-      <c r="N48" s="38"/>
+      <c r="L48" s="54"/>
+      <c r="M48" s="54"/>
+      <c r="N48" s="54"/>
       <c r="O48" s="27"/>
-      <c r="P48"/>
-    </row>
-    <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="27"/>
+      <c r="T48"/>
+    </row>
+    <row r="49" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2990,13 +3234,17 @@
       </c>
       <c r="G49" s="20"/>
       <c r="K49" s="20"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="38"/>
-      <c r="N49" s="38"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="54"/>
+      <c r="N49" s="54"/>
       <c r="O49" s="27"/>
-      <c r="P49"/>
-    </row>
-    <row r="50" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
+      <c r="S49" s="27"/>
+      <c r="T49"/>
+    </row>
+    <row r="50" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -3017,13 +3265,17 @@
       </c>
       <c r="G50" s="21"/>
       <c r="K50" s="21"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="38"/>
+      <c r="L50" s="54"/>
+      <c r="M50" s="54"/>
+      <c r="N50" s="54"/>
       <c r="O50" s="21"/>
-      <c r="P50"/>
-    </row>
-    <row r="51" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P50" s="38"/>
+      <c r="Q50" s="38"/>
+      <c r="R50" s="38"/>
+      <c r="S50" s="21"/>
+      <c r="T50"/>
+    </row>
+    <row r="51" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>219</v>
       </c>
@@ -3046,19 +3298,29 @@
         <v>302</v>
       </c>
       <c r="K51" s="21"/>
-      <c r="L51" s="47" t="s">
+      <c r="L51" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="M51" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="N51" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="O51" s="21"/>
+      <c r="P51" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="M51" s="47" t="s">
+      <c r="Q51" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="N51" s="47" t="s">
+      <c r="R51" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="O51" s="21"/>
-      <c r="P51"/>
-    </row>
-    <row r="52" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S51" s="21"/>
+      <c r="T51"/>
+    </row>
+    <row r="52" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
         <v>179</v>
       </c>
@@ -3080,9 +3342,10 @@
       <c r="G52" s="20"/>
       <c r="K52" s="20"/>
       <c r="O52" s="27"/>
-      <c r="P52"/>
-    </row>
-    <row r="53" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S52" s="27"/>
+      <c r="T52"/>
+    </row>
+    <row r="53" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
         <v>181</v>
       </c>
@@ -3104,9 +3367,10 @@
       <c r="G53" s="20"/>
       <c r="K53" s="20"/>
       <c r="O53" s="27"/>
-      <c r="P53"/>
-    </row>
-    <row r="54" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S53" s="27"/>
+      <c r="T53"/>
+    </row>
+    <row r="54" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -3127,13 +3391,17 @@
       </c>
       <c r="G54" s="20"/>
       <c r="K54" s="20"/>
-      <c r="L54" s="38"/>
-      <c r="M54" s="38"/>
-      <c r="N54" s="38"/>
+      <c r="L54" s="54"/>
+      <c r="M54" s="54"/>
+      <c r="N54" s="54"/>
       <c r="O54" s="27"/>
-      <c r="P54"/>
-    </row>
-    <row r="55" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P54" s="38"/>
+      <c r="Q54" s="38"/>
+      <c r="R54" s="38"/>
+      <c r="S54" s="27"/>
+      <c r="T54"/>
+    </row>
+    <row r="55" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -3154,13 +3422,17 @@
       </c>
       <c r="G55" s="20"/>
       <c r="K55" s="20"/>
-      <c r="L55" s="38"/>
-      <c r="M55" s="38"/>
-      <c r="N55" s="38"/>
+      <c r="L55" s="54"/>
+      <c r="M55" s="54"/>
+      <c r="N55" s="54"/>
       <c r="O55" s="27"/>
-      <c r="P55"/>
-    </row>
-    <row r="56" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
+      <c r="S55" s="27"/>
+      <c r="T55"/>
+    </row>
+    <row r="56" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
         <v>61</v>
       </c>
@@ -3182,9 +3454,10 @@
       <c r="G56" s="20"/>
       <c r="K56" s="20"/>
       <c r="O56" s="27"/>
-      <c r="P56"/>
-    </row>
-    <row r="57" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S56" s="27"/>
+      <c r="T56"/>
+    </row>
+    <row r="57" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>184</v>
       </c>
@@ -3205,13 +3478,17 @@
       </c>
       <c r="G57" s="20"/>
       <c r="K57" s="20"/>
-      <c r="L57" s="38"/>
-      <c r="M57" s="38"/>
-      <c r="N57" s="38"/>
+      <c r="L57" s="54"/>
+      <c r="M57" s="54"/>
+      <c r="N57" s="54"/>
       <c r="O57" s="27"/>
-      <c r="P57"/>
-    </row>
-    <row r="58" spans="1:16" s="51" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P57" s="38"/>
+      <c r="Q57" s="38"/>
+      <c r="R57" s="38"/>
+      <c r="S57" s="27"/>
+      <c r="T57"/>
+    </row>
+    <row r="58" spans="1:20" s="51" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="51" t="s">
         <v>315</v>
       </c>
@@ -3238,16 +3515,24 @@
         <v>4</v>
       </c>
       <c r="K58" s="27"/>
-      <c r="M58" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="N58" s="51" t="s">
+      <c r="L58" s="54"/>
+      <c r="M58" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N58" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O58" s="27"/>
-      <c r="P58"/>
-    </row>
-    <row r="59" spans="1:16" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Q58" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="R58" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="S58" s="27"/>
+      <c r="T58"/>
+    </row>
+    <row r="59" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
         <v>288</v>
       </c>
@@ -3273,9 +3558,11 @@
       <c r="K59" s="22"/>
       <c r="L59" s="16"/>
       <c r="O59" s="22"/>
-      <c r="P59"/>
-    </row>
-    <row r="60" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P59" s="16"/>
+      <c r="S59" s="22"/>
+      <c r="T59"/>
+    </row>
+    <row r="60" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
         <v>290</v>
       </c>
@@ -3297,8 +3584,9 @@
       <c r="G60" s="27"/>
       <c r="K60" s="27"/>
       <c r="O60" s="27"/>
-    </row>
-    <row r="61" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S60" s="27"/>
+    </row>
+    <row r="61" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
         <v>294</v>
       </c>
@@ -3323,8 +3611,9 @@
       <c r="J61" s="34"/>
       <c r="K61" s="27"/>
       <c r="O61" s="27"/>
-    </row>
-    <row r="62" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S61" s="27"/>
+    </row>
+    <row r="62" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
         <v>186</v>
       </c>
@@ -3343,9 +3632,10 @@
       <c r="G62" s="20"/>
       <c r="K62" s="20"/>
       <c r="O62" s="27"/>
-      <c r="P62"/>
-    </row>
-    <row r="63" spans="1:16" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S62" s="27"/>
+      <c r="T62"/>
+    </row>
+    <row r="63" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" s="16" t="s">
         <v>239</v>
       </c>
@@ -3373,9 +3663,13 @@
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
       <c r="O63" s="22"/>
-      <c r="P63"/>
-    </row>
-    <row r="64" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="22"/>
+      <c r="T63"/>
+    </row>
+    <row r="64" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
         <v>188</v>
       </c>
@@ -3397,9 +3691,10 @@
       <c r="G64" s="20"/>
       <c r="K64" s="20"/>
       <c r="O64" s="27"/>
-      <c r="P64"/>
-    </row>
-    <row r="65" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S64" s="27"/>
+      <c r="T64"/>
+    </row>
+    <row r="65" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -3420,13 +3715,17 @@
       </c>
       <c r="G65" s="20"/>
       <c r="K65" s="20"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="38"/>
+      <c r="L65" s="54"/>
+      <c r="M65" s="54"/>
+      <c r="N65" s="54"/>
       <c r="O65" s="27"/>
-      <c r="P65"/>
-    </row>
-    <row r="66" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P65" s="38"/>
+      <c r="Q65" s="38"/>
+      <c r="R65" s="38"/>
+      <c r="S65" s="27"/>
+      <c r="T65"/>
+    </row>
+    <row r="66" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -3448,9 +3747,10 @@
       <c r="G66" s="20"/>
       <c r="K66" s="20"/>
       <c r="O66" s="27"/>
-      <c r="P66"/>
-    </row>
-    <row r="67" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S66" s="27"/>
+      <c r="T66"/>
+    </row>
+    <row r="67" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>261</v>
       </c>
@@ -3472,9 +3772,10 @@
       <c r="G67" s="27"/>
       <c r="K67" s="27"/>
       <c r="O67" s="27"/>
-      <c r="P67"/>
-    </row>
-    <row r="68" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S67" s="27"/>
+      <c r="T67"/>
+    </row>
+    <row r="68" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -3495,13 +3796,17 @@
       </c>
       <c r="G68" s="20"/>
       <c r="K68" s="20"/>
-      <c r="L68" s="38"/>
-      <c r="M68" s="38"/>
-      <c r="N68" s="38"/>
+      <c r="L68" s="54"/>
+      <c r="M68" s="54"/>
+      <c r="N68" s="54"/>
       <c r="O68" s="27"/>
-      <c r="P68"/>
-    </row>
-    <row r="69" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P68" s="38"/>
+      <c r="Q68" s="38"/>
+      <c r="R68" s="38"/>
+      <c r="S68" s="27"/>
+      <c r="T68"/>
+    </row>
+    <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -3522,13 +3827,17 @@
       </c>
       <c r="G69" s="20"/>
       <c r="K69" s="20"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
+      <c r="L69" s="54"/>
+      <c r="M69" s="54"/>
+      <c r="N69" s="54"/>
       <c r="O69" s="27"/>
-      <c r="P69"/>
-    </row>
-    <row r="70" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P69" s="38"/>
+      <c r="Q69" s="38"/>
+      <c r="R69" s="38"/>
+      <c r="S69" s="27"/>
+      <c r="T69"/>
+    </row>
+    <row r="70" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -3549,13 +3858,17 @@
       </c>
       <c r="G70" s="20"/>
       <c r="K70" s="20"/>
-      <c r="L70" s="38"/>
-      <c r="M70" s="38"/>
-      <c r="N70" s="38"/>
+      <c r="L70" s="54"/>
+      <c r="M70" s="54"/>
+      <c r="N70" s="54"/>
       <c r="O70" s="27"/>
-      <c r="P70"/>
-    </row>
-    <row r="71" spans="1:17" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P70" s="38"/>
+      <c r="Q70" s="38"/>
+      <c r="R70" s="38"/>
+      <c r="S70" s="27"/>
+      <c r="T70"/>
+    </row>
+    <row r="71" spans="1:20" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="24" t="s">
         <v>253</v>
       </c>
@@ -3576,13 +3889,17 @@
       </c>
       <c r="G71" s="20"/>
       <c r="K71" s="20"/>
-      <c r="L71" s="38"/>
-      <c r="M71" s="38"/>
-      <c r="N71" s="38"/>
+      <c r="L71" s="54"/>
+      <c r="M71" s="54"/>
+      <c r="N71" s="54"/>
       <c r="O71" s="27"/>
-      <c r="P71"/>
-    </row>
-    <row r="72" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P71" s="38"/>
+      <c r="Q71" s="38"/>
+      <c r="R71" s="38"/>
+      <c r="S71" s="27"/>
+      <c r="T71"/>
+    </row>
+    <row r="72" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
@@ -3609,19 +3926,29 @@
         <v>302</v>
       </c>
       <c r="K72" s="21"/>
-      <c r="L72" s="47" t="s">
+      <c r="L72" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="M72" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="N72" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="O72" s="27"/>
+      <c r="P72" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="M72" s="47" t="s">
+      <c r="Q72" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="N72" s="47" t="s">
+      <c r="R72" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="O72" s="27"/>
-      <c r="P72"/>
-    </row>
-    <row r="73" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S72" s="27"/>
+      <c r="T72"/>
+    </row>
+    <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="46" t="s">
         <v>194</v>
       </c>
@@ -3640,13 +3967,17 @@
       <c r="F73" s="46"/>
       <c r="G73" s="20"/>
       <c r="K73" s="20"/>
-      <c r="L73" s="38"/>
-      <c r="M73" s="38"/>
-      <c r="N73" s="38"/>
+      <c r="L73" s="54"/>
+      <c r="M73" s="54"/>
+      <c r="N73" s="54"/>
       <c r="O73" s="27"/>
-      <c r="P73"/>
-    </row>
-    <row r="74" spans="1:17" s="52" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P73" s="38"/>
+      <c r="Q73" s="38"/>
+      <c r="R73" s="38"/>
+      <c r="S73" s="27"/>
+      <c r="T73"/>
+    </row>
+    <row r="74" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" s="52" t="s">
         <v>317</v>
       </c>
@@ -3667,10 +3998,14 @@
       </c>
       <c r="G74" s="27"/>
       <c r="K74" s="27"/>
+      <c r="L74" s="54"/>
+      <c r="M74" s="54"/>
+      <c r="N74" s="54"/>
       <c r="O74" s="27"/>
-      <c r="P74"/>
-    </row>
-    <row r="75" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S74" s="27"/>
+      <c r="T74"/>
+    </row>
+    <row r="75" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" s="7" t="s">
         <v>74</v>
       </c>
@@ -3692,9 +4027,10 @@
       <c r="G75" s="20"/>
       <c r="K75" s="20"/>
       <c r="O75" s="27"/>
-      <c r="P75"/>
-    </row>
-    <row r="76" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S75" s="27"/>
+      <c r="T75"/>
+    </row>
+    <row r="76" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="40" t="s">
         <v>311</v>
       </c>
@@ -3714,10 +4050,11 @@
         <v>4</v>
       </c>
       <c r="G76" s="27"/>
-      <c r="L76" s="27"/>
-      <c r="Q76" s="27"/>
-    </row>
-    <row r="77" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K76" s="27"/>
+      <c r="O76" s="27"/>
+      <c r="S76" s="27"/>
+    </row>
+    <row r="77" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>217</v>
       </c>
@@ -3738,13 +4075,17 @@
       </c>
       <c r="G77" s="20"/>
       <c r="K77" s="20"/>
-      <c r="L77" s="38"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="38"/>
+      <c r="L77" s="54"/>
+      <c r="M77" s="54"/>
+      <c r="N77" s="54"/>
       <c r="O77" s="27"/>
-      <c r="P77"/>
-    </row>
-    <row r="78" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P77" s="38"/>
+      <c r="Q77" s="38"/>
+      <c r="R77" s="38"/>
+      <c r="S77" s="27"/>
+      <c r="T77"/>
+    </row>
+    <row r="78" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -3765,13 +4106,17 @@
       </c>
       <c r="G78" s="20"/>
       <c r="K78" s="20"/>
-      <c r="L78" s="38"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="38"/>
+      <c r="L78" s="54"/>
+      <c r="M78" s="54"/>
+      <c r="N78" s="54"/>
       <c r="O78" s="27"/>
-      <c r="P78"/>
-    </row>
-    <row r="79" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P78" s="38"/>
+      <c r="Q78" s="38"/>
+      <c r="R78" s="38"/>
+      <c r="S78" s="27"/>
+      <c r="T78"/>
+    </row>
+    <row r="79" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -3799,19 +4144,29 @@
         <v>302</v>
       </c>
       <c r="K79" s="21"/>
-      <c r="L79" s="47" t="s">
+      <c r="L79" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="M79" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="N79" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="O79" s="27"/>
+      <c r="P79" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="M79" s="47" t="s">
+      <c r="Q79" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="N79" s="47" t="s">
+      <c r="R79" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="O79" s="27"/>
-      <c r="P79"/>
-    </row>
-    <row r="80" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S79" s="27"/>
+      <c r="T79"/>
+    </row>
+    <row r="80" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -3832,13 +4187,17 @@
       </c>
       <c r="G80" s="20"/>
       <c r="K80" s="20"/>
-      <c r="L80" s="38"/>
-      <c r="M80" s="38"/>
-      <c r="N80" s="38"/>
+      <c r="L80" s="54"/>
+      <c r="M80" s="54"/>
+      <c r="N80" s="54"/>
       <c r="O80" s="27"/>
-      <c r="P80"/>
-    </row>
-    <row r="81" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P80" s="38"/>
+      <c r="Q80" s="38"/>
+      <c r="R80" s="38"/>
+      <c r="S80" s="27"/>
+      <c r="T80"/>
+    </row>
+    <row r="81" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="7" t="s">
         <v>83</v>
       </c>
@@ -3860,9 +4219,10 @@
       <c r="G81" s="20"/>
       <c r="K81" s="20"/>
       <c r="O81" s="27"/>
-      <c r="P81"/>
-    </row>
-    <row r="82" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S81" s="27"/>
+      <c r="T81"/>
+    </row>
+    <row r="82" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>195</v>
       </c>
@@ -3883,13 +4243,17 @@
       </c>
       <c r="G82" s="20"/>
       <c r="K82" s="20"/>
-      <c r="L82" s="38"/>
-      <c r="M82" s="38"/>
-      <c r="N82" s="38"/>
+      <c r="L82" s="54"/>
+      <c r="M82" s="54"/>
+      <c r="N82" s="54"/>
       <c r="O82" s="27"/>
-      <c r="P82"/>
-    </row>
-    <row r="83" spans="1:16" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="P82" s="38"/>
+      <c r="Q82" s="38"/>
+      <c r="R82" s="38"/>
+      <c r="S82" s="27"/>
+      <c r="T82"/>
+    </row>
+    <row r="83" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
         <v>198</v>
       </c>
@@ -3911,9 +4275,10 @@
       <c r="G83" s="20"/>
       <c r="K83" s="20"/>
       <c r="O83" s="27"/>
-      <c r="P83"/>
-    </row>
-    <row r="84" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S83" s="27"/>
+      <c r="T83"/>
+    </row>
+    <row r="84" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>85</v>
       </c>
@@ -3940,19 +4305,29 @@
         <v>278</v>
       </c>
       <c r="K84" s="20"/>
-      <c r="L84" s="38" t="s">
+      <c r="L84" s="54" t="s">
+        <v>326</v>
+      </c>
+      <c r="M84" s="54" t="s">
+        <v>326</v>
+      </c>
+      <c r="N84" s="54" t="s">
+        <v>326</v>
+      </c>
+      <c r="O84" s="27"/>
+      <c r="P84" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="M84" s="38" t="s">
+      <c r="Q84" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="N84" s="38" t="s">
+      <c r="R84" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="O84" s="27"/>
-      <c r="P84"/>
-    </row>
-    <row r="85" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S84" s="27"/>
+      <c r="T84"/>
+    </row>
+    <row r="85" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>87</v>
       </c>
@@ -3973,13 +4348,17 @@
       </c>
       <c r="G85" s="20"/>
       <c r="K85" s="20"/>
-      <c r="L85" s="38"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
+      <c r="L85" s="54"/>
+      <c r="M85" s="54"/>
+      <c r="N85" s="54"/>
       <c r="O85" s="27"/>
-      <c r="P85"/>
-    </row>
-    <row r="86" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P85" s="38"/>
+      <c r="Q85" s="38"/>
+      <c r="R85" s="38"/>
+      <c r="S85" s="27"/>
+      <c r="T85"/>
+    </row>
+    <row r="86" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="7" t="s">
         <v>91</v>
       </c>
@@ -4001,9 +4380,10 @@
       <c r="G86" s="20"/>
       <c r="K86" s="20"/>
       <c r="O86" s="27"/>
-      <c r="P86"/>
-    </row>
-    <row r="87" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S86" s="27"/>
+      <c r="T86"/>
+    </row>
+    <row r="87" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
         <v>148</v>
       </c>
@@ -4025,9 +4405,10 @@
       <c r="G87" s="20"/>
       <c r="K87" s="20"/>
       <c r="O87" s="27"/>
-      <c r="P87"/>
-    </row>
-    <row r="88" spans="1:16" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="S87" s="27"/>
+      <c r="T87"/>
+    </row>
+    <row r="88" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -4048,13 +4429,17 @@
       </c>
       <c r="G88" s="20"/>
       <c r="K88" s="20"/>
-      <c r="L88" s="38"/>
-      <c r="M88" s="38"/>
-      <c r="N88" s="38"/>
+      <c r="L88" s="54"/>
+      <c r="M88" s="54"/>
+      <c r="N88" s="54"/>
       <c r="O88" s="27"/>
-      <c r="P88"/>
-    </row>
-    <row r="89" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P88" s="38"/>
+      <c r="Q88" s="38"/>
+      <c r="R88" s="38"/>
+      <c r="S88" s="27"/>
+      <c r="T88"/>
+    </row>
+    <row r="89" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>224</v>
       </c>
@@ -4077,19 +4462,29 @@
         <v>4</v>
       </c>
       <c r="K89" s="20"/>
-      <c r="L89" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M89" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N89" s="38" t="s">
+      <c r="L89" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M89" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="N89" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O89" s="27"/>
-      <c r="P89"/>
-    </row>
-    <row r="90" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P89" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q89" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="R89" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S89" s="27"/>
+      <c r="T89"/>
+    </row>
+    <row r="90" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>150</v>
       </c>
@@ -4110,13 +4505,17 @@
       </c>
       <c r="G90" s="20"/>
       <c r="K90" s="20"/>
-      <c r="L90" s="38"/>
-      <c r="M90" s="38"/>
-      <c r="N90" s="38"/>
+      <c r="L90" s="54"/>
+      <c r="M90" s="54"/>
+      <c r="N90" s="54"/>
       <c r="O90" s="27"/>
-      <c r="P90"/>
-    </row>
-    <row r="91" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P90" s="38"/>
+      <c r="Q90" s="38"/>
+      <c r="R90" s="38"/>
+      <c r="S90" s="27"/>
+      <c r="T90"/>
+    </row>
+    <row r="91" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="31" t="s">
         <v>98</v>
       </c>
@@ -4137,13 +4536,17 @@
       </c>
       <c r="G91" s="27"/>
       <c r="K91" s="27"/>
-      <c r="L91" s="38"/>
-      <c r="M91" s="38"/>
-      <c r="N91" s="38"/>
+      <c r="L91" s="54"/>
+      <c r="M91" s="54"/>
+      <c r="N91" s="54"/>
       <c r="O91" s="27"/>
-      <c r="P91"/>
-    </row>
-    <row r="92" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P91" s="38"/>
+      <c r="Q91" s="38"/>
+      <c r="R91" s="38"/>
+      <c r="S91" s="27"/>
+      <c r="T91"/>
+    </row>
+    <row r="92" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>200</v>
       </c>
@@ -4164,13 +4567,17 @@
       </c>
       <c r="G92" s="20"/>
       <c r="K92" s="20"/>
-      <c r="L92" s="38"/>
-      <c r="M92" s="38"/>
-      <c r="N92" s="38"/>
+      <c r="L92" s="54"/>
+      <c r="M92" s="54"/>
+      <c r="N92" s="54"/>
       <c r="O92" s="27"/>
-      <c r="P92"/>
-    </row>
-    <row r="93" spans="1:16" s="53" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P92" s="38"/>
+      <c r="Q92" s="38"/>
+      <c r="R92" s="38"/>
+      <c r="S92" s="27"/>
+      <c r="T92"/>
+    </row>
+    <row r="93" spans="1:20" s="53" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="53" t="s">
         <v>321</v>
       </c>
@@ -4197,10 +4604,14 @@
         <v>4</v>
       </c>
       <c r="K93" s="27"/>
+      <c r="L93" s="54"/>
+      <c r="M93" s="54"/>
+      <c r="N93" s="54"/>
       <c r="O93" s="27"/>
-      <c r="P93"/>
-    </row>
-    <row r="94" spans="1:16" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S93" s="27"/>
+      <c r="T93"/>
+    </row>
+    <row r="94" spans="1:20" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="14" t="s">
         <v>247</v>
       </c>
@@ -4221,13 +4632,17 @@
       </c>
       <c r="G94" s="20"/>
       <c r="K94" s="20"/>
-      <c r="L94" s="38"/>
-      <c r="M94" s="38"/>
-      <c r="N94" s="38"/>
+      <c r="L94" s="54"/>
+      <c r="M94" s="54"/>
+      <c r="N94" s="54"/>
       <c r="O94" s="27"/>
-      <c r="P94"/>
-    </row>
-    <row r="95" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P94" s="38"/>
+      <c r="Q94" s="38"/>
+      <c r="R94" s="38"/>
+      <c r="S94" s="27"/>
+      <c r="T94"/>
+    </row>
+    <row r="95" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>220</v>
       </c>
@@ -4246,13 +4661,17 @@
       <c r="I95" s="35"/>
       <c r="J95" s="35"/>
       <c r="K95" s="20"/>
-      <c r="L95" s="38"/>
-      <c r="M95" s="38"/>
-      <c r="N95" s="38"/>
+      <c r="L95" s="54"/>
+      <c r="M95" s="54"/>
+      <c r="N95" s="54"/>
       <c r="O95" s="27"/>
-      <c r="P95"/>
-    </row>
-    <row r="96" spans="1:16" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P95" s="38"/>
+      <c r="Q95" s="38"/>
+      <c r="R95" s="38"/>
+      <c r="S95" s="27"/>
+      <c r="T95"/>
+    </row>
+    <row r="96" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
@@ -4273,13 +4692,17 @@
       </c>
       <c r="G96" s="20"/>
       <c r="K96" s="20"/>
-      <c r="L96" s="38"/>
-      <c r="M96" s="38"/>
-      <c r="N96" s="38"/>
+      <c r="L96" s="54"/>
+      <c r="M96" s="54"/>
+      <c r="N96" s="54"/>
       <c r="O96" s="27"/>
-      <c r="P96"/>
-    </row>
-    <row r="97" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P96" s="38"/>
+      <c r="Q96" s="38"/>
+      <c r="R96" s="38"/>
+      <c r="S96" s="27"/>
+      <c r="T96"/>
+    </row>
+    <row r="97" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>284</v>
       </c>
@@ -4301,8 +4724,9 @@
       <c r="G97" s="27"/>
       <c r="K97" s="27"/>
       <c r="O97" s="27"/>
-    </row>
-    <row r="98" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S97" s="27"/>
+    </row>
+    <row r="98" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>102</v>
       </c>
@@ -4323,13 +4747,17 @@
       </c>
       <c r="G98" s="20"/>
       <c r="K98" s="20"/>
-      <c r="L98" s="38"/>
-      <c r="M98" s="38"/>
-      <c r="N98" s="38"/>
+      <c r="L98" s="54"/>
+      <c r="M98" s="54"/>
+      <c r="N98" s="54"/>
       <c r="O98" s="27"/>
-      <c r="P98"/>
-    </row>
-    <row r="99" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P98" s="38"/>
+      <c r="Q98" s="38"/>
+      <c r="R98" s="38"/>
+      <c r="S98" s="27"/>
+      <c r="T98"/>
+    </row>
+    <row r="99" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>104</v>
       </c>
@@ -4350,13 +4778,17 @@
       </c>
       <c r="G99" s="20"/>
       <c r="K99" s="20"/>
-      <c r="L99" s="38"/>
-      <c r="M99" s="38"/>
-      <c r="N99" s="38"/>
+      <c r="L99" s="54"/>
+      <c r="M99" s="54"/>
+      <c r="N99" s="54"/>
       <c r="O99" s="27"/>
-      <c r="P99"/>
-    </row>
-    <row r="100" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P99" s="38"/>
+      <c r="Q99" s="38"/>
+      <c r="R99" s="38"/>
+      <c r="S99" s="27"/>
+      <c r="T99"/>
+    </row>
+    <row r="100" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>203</v>
       </c>
@@ -4374,13 +4806,17 @@
       </c>
       <c r="G100" s="20"/>
       <c r="K100" s="20"/>
-      <c r="L100" s="38"/>
-      <c r="M100" s="38"/>
-      <c r="N100" s="38"/>
+      <c r="L100" s="54"/>
+      <c r="M100" s="54"/>
+      <c r="N100" s="54"/>
       <c r="O100" s="27"/>
-      <c r="P100"/>
-    </row>
-    <row r="101" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P100" s="38"/>
+      <c r="Q100" s="38"/>
+      <c r="R100" s="38"/>
+      <c r="S100" s="27"/>
+      <c r="T100"/>
+    </row>
+    <row r="101" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>106</v>
       </c>
@@ -4401,13 +4837,17 @@
       </c>
       <c r="G101" s="20"/>
       <c r="K101" s="20"/>
-      <c r="L101" s="38"/>
-      <c r="M101" s="38"/>
-      <c r="N101" s="38"/>
+      <c r="L101" s="54"/>
+      <c r="M101" s="54"/>
+      <c r="N101" s="54"/>
       <c r="O101" s="27"/>
-      <c r="P101"/>
-    </row>
-    <row r="102" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P101" s="38"/>
+      <c r="Q101" s="38"/>
+      <c r="R101" s="38"/>
+      <c r="S101" s="27"/>
+      <c r="T101"/>
+    </row>
+    <row r="102" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>110</v>
       </c>
@@ -4434,19 +4874,29 @@
         <v>302</v>
       </c>
       <c r="K102" s="21"/>
-      <c r="L102" s="47" t="s">
+      <c r="L102" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="M102" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="N102" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="O102" s="27"/>
+      <c r="P102" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="M102" s="47" t="s">
+      <c r="Q102" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="N102" s="47" t="s">
+      <c r="R102" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="O102" s="27"/>
-      <c r="P102"/>
-    </row>
-    <row r="103" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S102" s="27"/>
+      <c r="T102"/>
+    </row>
+    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="7" t="s">
         <v>112</v>
       </c>
@@ -4468,9 +4918,10 @@
       <c r="G103" s="20"/>
       <c r="K103" s="20"/>
       <c r="O103" s="27"/>
-      <c r="P103"/>
-    </row>
-    <row r="104" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S103" s="27"/>
+      <c r="T103"/>
+    </row>
+    <row r="104" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="7" t="s">
         <v>114</v>
       </c>
@@ -4492,9 +4943,10 @@
       <c r="G104" s="20"/>
       <c r="K104" s="20"/>
       <c r="O104" s="27"/>
-      <c r="P104"/>
-    </row>
-    <row r="105" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S104" s="27"/>
+      <c r="T104"/>
+    </row>
+    <row r="105" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="7" t="s">
         <v>116</v>
       </c>
@@ -4516,9 +4968,10 @@
       <c r="G105" s="20"/>
       <c r="K105" s="20"/>
       <c r="O105" s="27"/>
-      <c r="P105"/>
-    </row>
-    <row r="106" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S105" s="27"/>
+      <c r="T105"/>
+    </row>
+    <row r="106" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>118</v>
       </c>
@@ -4545,19 +4998,29 @@
         <v>4</v>
       </c>
       <c r="K106" s="20"/>
-      <c r="L106" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="M106" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N106" s="38" t="s">
+      <c r="L106" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="M106" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N106" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O106" s="27"/>
-      <c r="P106"/>
-    </row>
-    <row r="107" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P106" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q106" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R106" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S106" s="27"/>
+      <c r="T106"/>
+    </row>
+    <row r="107" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>120</v>
       </c>
@@ -4584,19 +5047,29 @@
         <v>4</v>
       </c>
       <c r="K107" s="20"/>
-      <c r="L107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="M107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N107" s="38" t="s">
+      <c r="L107" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="M107" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N107" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O107" s="27"/>
-      <c r="P107"/>
-    </row>
-    <row r="108" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P107" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q107" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R107" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S107" s="27"/>
+      <c r="T107"/>
+    </row>
+    <row r="108" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>122</v>
       </c>
@@ -4623,19 +5096,29 @@
         <v>4</v>
       </c>
       <c r="K108" s="20"/>
-      <c r="L108" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M108" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N108" s="38" t="s">
+      <c r="L108" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M108" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N108" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O108" s="27"/>
-      <c r="P108"/>
-    </row>
-    <row r="109" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P108" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q108" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R108" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S108" s="27"/>
+      <c r="T108"/>
+    </row>
+    <row r="109" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>152</v>
       </c>
@@ -4659,13 +5142,17 @@
       <c r="I109"/>
       <c r="J109"/>
       <c r="K109" s="20"/>
-      <c r="L109" s="38"/>
-      <c r="M109" s="38"/>
-      <c r="N109" s="38"/>
+      <c r="L109" s="54"/>
+      <c r="M109" s="54"/>
+      <c r="N109" s="54"/>
       <c r="O109" s="27"/>
-      <c r="P109"/>
-    </row>
-    <row r="110" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P109" s="38"/>
+      <c r="Q109" s="38"/>
+      <c r="R109" s="38"/>
+      <c r="S109" s="27"/>
+      <c r="T109"/>
+    </row>
+    <row r="110" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>286</v>
       </c>
@@ -4693,8 +5180,12 @@
       <c r="M110"/>
       <c r="N110"/>
       <c r="O110" s="27"/>
-    </row>
-    <row r="111" spans="1:16" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P110"/>
+      <c r="Q110"/>
+      <c r="R110"/>
+      <c r="S110" s="27"/>
+    </row>
+    <row r="111" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A111" s="7" t="s">
         <v>124</v>
       </c>
@@ -4716,8 +5207,9 @@
       <c r="G111" s="20"/>
       <c r="K111" s="20"/>
       <c r="O111" s="27"/>
-    </row>
-    <row r="112" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S111" s="27"/>
+    </row>
+    <row r="112" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>127</v>
       </c>
@@ -4744,18 +5236,28 @@
         <v>4</v>
       </c>
       <c r="K112" s="20"/>
-      <c r="L112" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M112" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N112" s="38" t="s">
+      <c r="L112" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M112" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N112" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O112" s="27"/>
-    </row>
-    <row r="113" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P112" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q112" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R112" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S112" s="27"/>
+    </row>
+    <row r="113" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>238</v>
       </c>
@@ -4782,18 +5284,28 @@
         <v>4</v>
       </c>
       <c r="K113" s="20"/>
-      <c r="L113" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="M113" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N113" s="38" t="s">
+      <c r="L113" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="M113" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="N113" s="54" t="s">
         <v>4</v>
       </c>
       <c r="O113" s="27"/>
-    </row>
-    <row r="114" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P113" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="R113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S113" s="27"/>
+    </row>
+    <row r="114" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>130</v>
       </c>
@@ -4814,12 +5326,16 @@
       </c>
       <c r="G114" s="20"/>
       <c r="K114" s="20"/>
-      <c r="L114" s="38"/>
-      <c r="M114" s="38"/>
-      <c r="N114" s="38"/>
+      <c r="L114" s="54"/>
+      <c r="M114" s="54"/>
+      <c r="N114" s="54"/>
       <c r="O114" s="27"/>
-    </row>
-    <row r="115" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P114" s="38"/>
+      <c r="Q114" s="38"/>
+      <c r="R114" s="38"/>
+      <c r="S114" s="27"/>
+    </row>
+    <row r="115" spans="1:20" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="48" t="s">
         <v>307</v>
       </c>
@@ -4846,18 +5362,28 @@
         <v>309</v>
       </c>
       <c r="K115" s="21"/>
-      <c r="L115" s="48" t="s">
+      <c r="L115" s="54" t="s">
+        <v>328</v>
+      </c>
+      <c r="M115" s="54" t="s">
+        <v>328</v>
+      </c>
+      <c r="N115" s="54" t="s">
+        <v>328</v>
+      </c>
+      <c r="O115" s="27"/>
+      <c r="P115" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="M115" s="48" t="s">
+      <c r="Q115" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="N115" s="48" t="s">
+      <c r="R115" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="O115" s="27"/>
-    </row>
-    <row r="116" spans="1:16" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="S115" s="27"/>
+    </row>
+    <row r="116" spans="1:20" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A116" s="26" t="s">
         <v>256</v>
       </c>
@@ -4881,12 +5407,16 @@
       <c r="I116" s="26"/>
       <c r="J116" s="26"/>
       <c r="K116" s="27"/>
-      <c r="L116" s="38"/>
-      <c r="M116" s="38"/>
-      <c r="N116" s="38"/>
+      <c r="L116" s="54"/>
+      <c r="M116" s="54"/>
+      <c r="N116" s="54"/>
       <c r="O116" s="27"/>
-    </row>
-    <row r="117" spans="1:16" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="P116" s="38"/>
+      <c r="Q116" s="38"/>
+      <c r="R116" s="38"/>
+      <c r="S116" s="27"/>
+    </row>
+    <row r="117" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>132</v>
       </c>
@@ -4907,76 +5437,80 @@
       </c>
       <c r="G117" s="20"/>
       <c r="K117" s="20"/>
-      <c r="L117" s="38"/>
-      <c r="M117" s="38"/>
-      <c r="N117" s="38"/>
+      <c r="L117" s="54"/>
+      <c r="M117" s="54"/>
+      <c r="N117" s="54"/>
       <c r="O117" s="27"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P118"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P119"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P120"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P121"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P122"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P123"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P124"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P125"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P126"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P127"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="P128"/>
-    </row>
-    <row r="129" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P129"/>
-    </row>
-    <row r="130" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P130"/>
-    </row>
-    <row r="131" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P131"/>
-    </row>
-    <row r="132" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P132"/>
-    </row>
-    <row r="133" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P133"/>
-    </row>
-    <row r="134" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P134"/>
-    </row>
-    <row r="135" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P135"/>
-    </row>
-    <row r="136" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P136"/>
-    </row>
-    <row r="137" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P137"/>
-    </row>
-    <row r="138" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P138"/>
-    </row>
-    <row r="139" spans="16:16" x14ac:dyDescent="0.4">
-      <c r="P139"/>
+      <c r="P117" s="38"/>
+      <c r="Q117" s="38"/>
+      <c r="R117" s="38"/>
+      <c r="S117" s="27"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T118"/>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T119"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T120"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T121"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T122"/>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T123"/>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T124"/>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T125"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T126"/>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T127"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T128"/>
+    </row>
+    <row r="129" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T129"/>
+    </row>
+    <row r="130" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T130"/>
+    </row>
+    <row r="131" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T131"/>
+    </row>
+    <row r="132" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T132"/>
+    </row>
+    <row r="133" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T133"/>
+    </row>
+    <row r="134" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T134"/>
+    </row>
+    <row r="135" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T135"/>
+    </row>
+    <row r="136" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T136"/>
+    </row>
+    <row r="137" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T137"/>
+    </row>
+    <row r="138" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T138"/>
+    </row>
+    <row r="139" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T139"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[WK] naam conceptuel schema aangepast
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -927,9 +927,6 @@
     <t>20200801</t>
   </si>
   <si>
-    <t>Waarderingskamer_GEOSTANDAARDEN</t>
-  </si>
-  <si>
     <t>WaarderingskamerBSM</t>
   </si>
   <si>
@@ -1012,6 +1009,9 @@
   </si>
   <si>
     <t>WKUGM</t>
+  </si>
+  <si>
+    <t>NEN3610_GML321</t>
   </si>
 </sst>
 </file>
@@ -1603,10 +1603,10 @@
   <dimension ref="A1:T139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H102" sqref="H102"/>
+      <selection pane="bottomRight" activeCell="H69" sqref="H69:H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1700,13 +1700,13 @@
       </c>
       <c r="K2" s="19"/>
       <c r="L2" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>325</v>
       </c>
       <c r="O2" s="19"/>
       <c r="P2" s="3" t="s">
@@ -2232,7 +2232,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G20" s="20"/>
       <c r="K20" s="20"/>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G21" s="20"/>
       <c r="K21" s="20"/>
@@ -2479,13 +2479,13 @@
     </row>
     <row r="27" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B27" s="50" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D27" s="50" t="b">
         <v>0</v>
@@ -2889,13 +2889,13 @@
     </row>
     <row r="38" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="52" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B38" s="52" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="52" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D38" s="52" t="b">
         <v>0</v>
@@ -3289,33 +3289,33 @@
       </c>
       <c r="G51" s="21"/>
       <c r="H51" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I51" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J51" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K51" s="21"/>
       <c r="L51" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M51" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N51" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O51" s="21"/>
       <c r="P51" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q51" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R51" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S51" s="21"/>
       <c r="T51"/>
@@ -3490,13 +3490,13 @@
     </row>
     <row r="58" spans="1:20" s="51" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B58" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D58" s="51" t="b">
         <v>0</v>
@@ -3549,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="16"/>
@@ -3603,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G61" s="27"/>
       <c r="H61" s="34"/>
@@ -3806,7 +3806,7 @@
       <c r="S68" s="27"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="G69" s="20"/>
       <c r="K69" s="20"/>
@@ -3917,33 +3917,33 @@
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I72" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J72" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K72" s="21"/>
       <c r="L72" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M72" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N72" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O72" s="27"/>
       <c r="P72" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q72" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R72" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S72" s="27"/>
       <c r="T72"/>
@@ -3979,13 +3979,13 @@
     </row>
     <row r="74" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" s="52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B74" s="52" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D74" s="52" t="b">
         <v>0</v>
@@ -4032,13 +4032,13 @@
     </row>
     <row r="76" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B76" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D76" s="49" t="b">
         <v>0</v>
@@ -4135,33 +4135,33 @@
       <c r="F79" s="33"/>
       <c r="G79" s="20"/>
       <c r="H79" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I79" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J79" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K79" s="21"/>
       <c r="L79" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M79" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N79" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O79" s="27"/>
       <c r="P79" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q79" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R79" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S79" s="27"/>
       <c r="T79"/>
@@ -4306,13 +4306,13 @@
       </c>
       <c r="K84" s="20"/>
       <c r="L84" s="54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M84" s="54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N84" s="54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O84" s="27"/>
       <c r="P84" s="38" t="s">
@@ -4579,13 +4579,13 @@
     </row>
     <row r="93" spans="1:20" s="53" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="53" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B93" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="53" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D93" s="53" t="b">
         <v>0</v>
@@ -4865,33 +4865,33 @@
       </c>
       <c r="G102" s="20"/>
       <c r="H102" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I102" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J102" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K102" s="21"/>
       <c r="L102" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M102" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N102" s="54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O102" s="27"/>
       <c r="P102" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q102" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R102" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S102" s="27"/>
       <c r="T102"/>
@@ -5337,13 +5337,13 @@
     </row>
     <row r="115" spans="1:20" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B115" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D115" s="48" t="b">
         <v>1</v>
@@ -5353,33 +5353,33 @@
       </c>
       <c r="G115" s="27"/>
       <c r="H115" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I115" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J115" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K115" s="21"/>
       <c r="L115" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M115" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N115" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O115" s="27"/>
       <c r="P115" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q115" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R115" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S115" s="27"/>
     </row>

</xml_diff>

<commit_message>
[waarderingskamer] activeer YAML compiler (OpenAPI)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -1603,10 +1603,10 @@
   <dimension ref="A1:T139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H69" sqref="H69:H70"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2674,7 +2674,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="31"/>

</xml_diff>

<commit_message>
[WK] nativescalars = no
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -1603,10 +1603,10 @@
   <dimension ref="A1:T139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4047,7 +4047,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="49" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G76" s="27"/>
       <c r="K76" s="27"/>

</xml_diff>

<commit_message>
XHTML respec catalogus genereren naast bestaande HTML
Resulteert in *.respec.catalog.xhtml. Deze catalogus kan als XML worden
opgepikt om te integreren in documentatie.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="329">
   <si>
     <t>Name</t>
   </si>
@@ -1603,10 +1603,10 @@
   <dimension ref="A1:T139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G76" sqref="G76"/>
+      <selection pane="bottomRight" activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1621,9 +1621,9 @@
     <col min="8" max="9" width="14.765625" customWidth="1"/>
     <col min="10" max="10" width="14.3046875" customWidth="1"/>
     <col min="11" max="11" width="5.4609375" style="23" customWidth="1"/>
-    <col min="12" max="12" width="28.3046875" customWidth="1"/>
-    <col min="13" max="13" width="25.3828125" customWidth="1"/>
-    <col min="14" max="14" width="26.921875" customWidth="1"/>
+    <col min="12" max="12" width="11.84375" customWidth="1"/>
+    <col min="13" max="13" width="14.3828125" customWidth="1"/>
+    <col min="14" max="14" width="16.921875" customWidth="1"/>
     <col min="15" max="15" width="5.4609375" style="23" customWidth="1"/>
     <col min="16" max="16" width="16.15234375" customWidth="1"/>
     <col min="17" max="17" width="16.07421875" customWidth="1"/>
@@ -3508,27 +3508,11 @@
         <v>16</v>
       </c>
       <c r="G58" s="27"/>
-      <c r="I58" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="J58" s="51" t="s">
-        <v>4</v>
-      </c>
       <c r="K58" s="27"/>
       <c r="L58" s="54"/>
-      <c r="M58" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="N58" s="54" t="s">
-        <v>4</v>
-      </c>
+      <c r="M58" s="54"/>
+      <c r="N58" s="54"/>
       <c r="O58" s="27"/>
-      <c r="Q58" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="R58" s="51" t="s">
-        <v>4</v>
-      </c>
       <c r="S58" s="27"/>
       <c r="T58"/>
     </row>

</xml_diff>

<commit_message>
WK: Aanpassingen modeldocumentatie: weergave data locatie
De data locatie wordt nu ook getoond bij de inhoud van de waardelijsten,
onder de definitie.
Kopjes worden niet meer getoond als er geen data wordt uitgelezen uit
een waardenlijst bron locatie.

Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
+++ b/src/main/resources/input/Waarderingskamer/props/Waarderingskamer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Waarderingskamer\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889FF3FF-7A9B-443C-88C9-0894E41C23A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855AAEDF-788C-45CC-866E-E7CCC98FCDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="345">
   <si>
     <t>Name</t>
   </si>
@@ -835,9 +835,6 @@
     <t>click</t>
   </si>
   <si>
-    <t>[project-name]-[application-name]-[phase]-[release]</t>
-  </si>
-  <si>
     <t>createofficevariant</t>
   </si>
   <si>
@@ -847,9 +844,6 @@
     <t>Specify the type of office file. Multiple formats are allowed, separate list by whitespace.</t>
   </si>
   <si>
-    <t>respec</t>
-  </si>
-  <si>
     <t>SIM: opleveren</t>
   </si>
   <si>
@@ -1058,6 +1052,15 @@
   </si>
   <si>
     <t>Vetsion of the extension. When this is a MIM model, specify the MIM extension version</t>
+  </si>
+  <si>
+    <t>documentor</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>includedoclist</t>
   </si>
 </sst>
 </file>
@@ -1550,13 +1553,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W144"/>
+  <dimension ref="A1:W145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F75" sqref="F75"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1652,42 +1655,42 @@
       <c r="F2" s="3"/>
       <c r="G2" s="15"/>
       <c r="H2" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="U2" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="V2" s="15"/>
       <c r="W2" s="5"/>
@@ -2087,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G18" s="16"/>
       <c r="L18" s="16"/>
@@ -2134,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G20" s="16"/>
       <c r="L20" s="16"/>
@@ -2159,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G21" s="16"/>
       <c r="L21" s="16"/>
@@ -2390,13 +2393,13 @@
     </row>
     <row r="27" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
@@ -2604,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G31" s="16"/>
       <c r="L31" s="16"/>
@@ -2722,14 +2725,14 @@
     </row>
     <row r="35" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>273</v>
+        <v>342</v>
       </c>
       <c r="G35" s="16"/>
       <c r="L35" s="16"/>
@@ -2771,13 +2774,13 @@
     </row>
     <row r="37" spans="1:23" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D37" s="21" t="b">
         <v>0</v>
@@ -2795,13 +2798,13 @@
     </row>
     <row r="38" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
@@ -2909,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G42" s="16"/>
       <c r="L42" s="16"/>
@@ -3144,42 +3147,42 @@
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L51" s="17"/>
       <c r="M51" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Q51" s="17"/>
       <c r="R51" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="V51" s="17"/>
       <c r="W51"/>
@@ -3336,13 +3339,13 @@
     </row>
     <row r="58" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D58" s="2" t="b">
         <v>0</v>
@@ -3361,13 +3364,13 @@
     </row>
     <row r="59" spans="1:23" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D59" s="13" t="b">
         <v>0</v>
@@ -3376,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="13"/>
@@ -3392,22 +3395,22 @@
     </row>
     <row r="60" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>291</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="G60" s="16"/>
       <c r="L60" s="16"/>
@@ -3416,13 +3419,13 @@
     </row>
     <row r="61" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -3431,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="20"/>
@@ -3551,24 +3554,21 @@
       <c r="V65" s="16"/>
       <c r="W65"/>
     </row>
-    <row r="66" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D66" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>218</v>
+    <row r="66" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G66" s="16"/>
       <c r="L66" s="16"/>
@@ -3577,23 +3577,23 @@
       <c r="W66"/>
     </row>
     <row r="67" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>261</v>
-      </c>
-      <c r="B67" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" t="s">
-        <v>262</v>
-      </c>
-      <c r="D67" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>226</v>
+      <c r="A67" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="G67" s="16"/>
       <c r="L67" s="16"/>
@@ -3601,24 +3601,24 @@
       <c r="V67" s="16"/>
       <c r="W67"/>
     </row>
-    <row r="68" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>210</v>
+    <row r="68" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>261</v>
+      </c>
+      <c r="B68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" t="s">
+        <v>262</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>226</v>
       </c>
       <c r="G68" s="16"/>
       <c r="L68" s="16"/>
@@ -3626,15 +3626,15 @@
       <c r="V68" s="16"/>
       <c r="W68"/>
     </row>
-    <row r="69" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
@@ -3643,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>328</v>
+        <v>210</v>
       </c>
       <c r="G69" s="16"/>
       <c r="L69" s="16"/>
@@ -3651,24 +3651,24 @@
       <c r="V69" s="16"/>
       <c r="W69"/>
     </row>
-    <row r="70" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="D70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E70" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>208</v>
+        <v>326</v>
       </c>
       <c r="G70" s="16"/>
       <c r="L70" s="16"/>
@@ -3678,13 +3678,13 @@
     </row>
     <row r="71" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>253</v>
+        <v>191</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>255</v>
+        <v>193</v>
       </c>
       <c r="D71" s="2" t="b">
         <v>0</v>
@@ -3693,7 +3693,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>254</v>
+        <v>208</v>
       </c>
       <c r="G71" s="16"/>
       <c r="L71" s="16"/>
@@ -3701,61 +3701,62 @@
       <c r="V71" s="16"/>
       <c r="W71"/>
     </row>
-    <row r="72" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>253</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>73</v>
+        <v>255</v>
       </c>
       <c r="D72" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="G72" s="16"/>
-      <c r="L72" s="17"/>
+      <c r="L72" s="16"/>
       <c r="Q72" s="16"/>
       <c r="V72" s="16"/>
       <c r="W72"/>
     </row>
-    <row r="73" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>334</v>
+        <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>335</v>
+        <v>73</v>
       </c>
       <c r="D73" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>336</v>
+        <v>0</v>
       </c>
       <c r="G73" s="16"/>
       <c r="L73" s="17"/>
       <c r="Q73" s="16"/>
       <c r="V73" s="16"/>
+      <c r="W73"/>
     </row>
     <row r="74" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>240</v>
+        <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3764,7 +3765,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G74" s="16"/>
       <c r="L74" s="17"/>
@@ -3773,13 +3774,13 @@
     </row>
     <row r="75" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>240</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3787,56 +3788,23 @@
       <c r="E75" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F75" s="2" t="s">
+        <v>337</v>
+      </c>
       <c r="G75" s="16"/>
-      <c r="H75" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="L75" s="17"/>
-      <c r="M75" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="N75" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="P75" s="2" t="s">
-        <v>325</v>
-      </c>
       <c r="Q75" s="16"/>
-      <c r="R75" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="S75" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="T75" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="U75" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="V75" s="16"/>
     </row>
     <row r="76" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>240</v>
+        <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -3845,19 +3813,55 @@
         <v>1</v>
       </c>
       <c r="G76" s="16"/>
+      <c r="H76" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="L76" s="17"/>
+      <c r="M76" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="P76" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="Q76" s="16"/>
+      <c r="R76" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="S76" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="T76" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="U76" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="V76" s="16"/>
     </row>
     <row r="77" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>194</v>
+        <v>340</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>10</v>
+        <v>240</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>297</v>
+        <v>341</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
@@ -3866,29 +3870,25 @@
         <v>1</v>
       </c>
       <c r="G77" s="16"/>
-      <c r="L77" s="16"/>
+      <c r="L77" s="17"/>
       <c r="Q77" s="16"/>
       <c r="V77" s="16"/>
-      <c r="W77"/>
-    </row>
-    <row r="78" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="78" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>316</v>
+        <v>194</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="G78" s="16"/>
       <c r="L78" s="16"/>
@@ -3896,24 +3896,24 @@
       <c r="V78" s="16"/>
       <c r="W78"/>
     </row>
-    <row r="79" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>4</v>
+    <row r="79" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G79" s="16"/>
       <c r="L79" s="16"/>
@@ -3921,45 +3921,46 @@
       <c r="V79" s="16"/>
       <c r="W79"/>
     </row>
-    <row r="80" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="B80" s="21" t="s">
+    <row r="80" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>16</v>
+      <c r="C80" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="G80" s="16"/>
       <c r="L80" s="16"/>
       <c r="Q80" s="16"/>
       <c r="V80" s="16"/>
-    </row>
-    <row r="81" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B81" s="2" t="s">
+      <c r="W80"/>
+    </row>
+    <row r="81" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="B81" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>229</v>
+      <c r="C81" s="21" t="s">
+        <v>309</v>
       </c>
       <c r="D81" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>16</v>
@@ -3968,26 +3969,25 @@
       <c r="L81" s="16"/>
       <c r="Q81" s="16"/>
       <c r="V81" s="16"/>
-      <c r="W81"/>
     </row>
     <row r="82" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>77</v>
+        <v>229</v>
       </c>
       <c r="D82" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G82" s="16"/>
       <c r="L82" s="16"/>
@@ -3997,105 +3997,105 @@
     </row>
     <row r="83" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D83" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F83" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G83" s="16"/>
-      <c r="H83" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="L83" s="17"/>
-      <c r="M83" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="N83" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="O83" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="P83" s="2" t="s">
-        <v>326</v>
-      </c>
+      <c r="L83" s="16"/>
       <c r="Q83" s="16"/>
-      <c r="R83" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="S83" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="T83" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="U83" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="V83" s="16"/>
       <c r="W83"/>
     </row>
     <row r="84" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D84" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F84" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="G84" s="16"/>
-      <c r="L84" s="16"/>
+      <c r="H84" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L84" s="17"/>
+      <c r="M84" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="N84" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="O84" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="P84" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="Q84" s="16"/>
+      <c r="R84" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="S84" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="T84" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="U84" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="V84" s="16"/>
       <c r="W84"/>
     </row>
-    <row r="85" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>298</v>
+    <row r="85" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="G85" s="16"/>
       <c r="L85" s="16"/>
@@ -4103,24 +4103,24 @@
       <c r="V85" s="16"/>
       <c r="W85"/>
     </row>
-    <row r="86" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>19</v>
+    <row r="86" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="G86" s="16"/>
       <c r="L86" s="16"/>
@@ -4128,24 +4128,24 @@
       <c r="V86" s="16"/>
       <c r="W86"/>
     </row>
-    <row r="87" spans="1:23" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>211</v>
+    <row r="87" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G87" s="16"/>
       <c r="L87" s="16"/>
@@ -4153,107 +4153,107 @@
       <c r="V87" s="16"/>
       <c r="W87"/>
     </row>
-    <row r="88" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>0</v>
+    <row r="88" spans="1:23" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="G88" s="16"/>
-      <c r="H88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="L88" s="16"/>
-      <c r="M88" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="N88" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="O88" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="P88" s="2" t="s">
-        <v>325</v>
-      </c>
       <c r="Q88" s="16"/>
-      <c r="R88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="S88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="T88" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="U88" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="V88" s="16"/>
       <c r="W88"/>
     </row>
     <row r="89" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G89" s="16"/>
+      <c r="H89" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="L89" s="16"/>
+      <c r="M89" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="N89" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="O89" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="P89" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="Q89" s="16"/>
+      <c r="R89" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="T89" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="U89" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="V89" s="16"/>
       <c r="W89"/>
     </row>
-    <row r="90" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D90" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>92</v>
+    <row r="90" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="G90" s="16"/>
       <c r="L90" s="16"/>
@@ -4263,22 +4263,22 @@
     </row>
     <row r="91" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A91" s="7" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D91" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="G91" s="16"/>
       <c r="L91" s="16"/>
@@ -4287,170 +4287,170 @@
       <c r="W91"/>
     </row>
     <row r="92" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="21" t="s">
-        <v>332</v>
-      </c>
-      <c r="B92" s="21" t="s">
+      <c r="A92" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="21" t="s">
-        <v>333</v>
-      </c>
-      <c r="D92" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="22"/>
-      <c r="H92" s="21"/>
-      <c r="I92" s="21"/>
-      <c r="J92" s="21"/>
-      <c r="K92" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="L92" s="22"/>
-      <c r="M92" s="21"/>
-      <c r="N92" s="21"/>
-      <c r="O92" s="21"/>
-      <c r="P92" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q92" s="22"/>
-      <c r="R92" s="21"/>
-      <c r="S92" s="21"/>
-      <c r="T92" s="21"/>
-      <c r="U92" s="21" t="s">
-        <v>4</v>
-      </c>
+      <c r="C92" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="16"/>
+      <c r="L92" s="16"/>
+      <c r="Q92" s="16"/>
       <c r="V92" s="16"/>
       <c r="W92"/>
     </row>
-    <row r="93" spans="1:23" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G93" s="16"/>
-      <c r="L93" s="16"/>
-      <c r="Q93" s="16"/>
+    <row r="93" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="D93" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="22"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L93" s="22"/>
+      <c r="M93" s="21"/>
+      <c r="N93" s="21"/>
+      <c r="O93" s="21"/>
+      <c r="P93" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q93" s="22"/>
+      <c r="R93" s="21"/>
+      <c r="S93" s="21"/>
+      <c r="T93" s="21"/>
+      <c r="U93" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="V93" s="16"/>
       <c r="W93"/>
     </row>
-    <row r="94" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:23" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D94" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G94" s="16"/>
-      <c r="H94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K94" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="L94" s="16"/>
-      <c r="M94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P94" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="Q94" s="16"/>
-      <c r="R94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S94" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U94" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="V94" s="16"/>
       <c r="W94"/>
     </row>
     <row r="95" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
       <c r="D95" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G95" s="16"/>
+      <c r="H95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L95" s="16"/>
+      <c r="M95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P95" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="Q95" s="16"/>
+      <c r="R95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U95" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="V95" s="16"/>
       <c r="W95"/>
     </row>
     <row r="96" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>267</v>
+        <v>4</v>
       </c>
       <c r="G96" s="16"/>
       <c r="L96" s="16"/>
@@ -4458,24 +4458,24 @@
       <c r="V96" s="16"/>
       <c r="W96"/>
     </row>
-    <row r="97" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>200</v>
+        <v>98</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>201</v>
+        <v>10</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
       <c r="D97" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="G97" s="16"/>
       <c r="L97" s="16"/>
@@ -4485,13 +4485,13 @@
     </row>
     <row r="98" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>320</v>
+        <v>200</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
@@ -4500,18 +4500,9 @@
         <v>1</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>16</v>
+        <v>251</v>
       </c>
       <c r="G98" s="16"/>
-      <c r="I98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L98" s="16"/>
       <c r="Q98" s="16"/>
       <c r="V98" s="16"/>
@@ -4519,13 +4510,13 @@
     </row>
     <row r="99" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>247</v>
+        <v>318</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>248</v>
+        <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>249</v>
+        <v>319</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>0</v>
@@ -4533,29 +4524,42 @@
       <c r="E99" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F99" s="6" t="s">
-        <v>250</v>
+      <c r="F99" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G99" s="16"/>
+      <c r="I99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L99" s="16"/>
       <c r="Q99" s="16"/>
       <c r="V99" s="16"/>
       <c r="W99"/>
     </row>
-    <row r="100" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
+        <v>247</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>249</v>
+      </c>
       <c r="D100" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F100" s="2" t="s">
-        <v>298</v>
+      <c r="F100" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="G100" s="16"/>
       <c r="L100" s="16"/>
@@ -4563,24 +4567,20 @@
       <c r="V100" s="16"/>
       <c r="W100"/>
     </row>
-    <row r="101" spans="1:23" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
       <c r="D101" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>16</v>
+        <v>296</v>
       </c>
       <c r="G101" s="16"/>
       <c r="L101" s="16"/>
@@ -4588,64 +4588,64 @@
       <c r="V101" s="16"/>
       <c r="W101"/>
     </row>
-    <row r="102" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" t="s">
-        <v>284</v>
-      </c>
-      <c r="B102" t="s">
-        <v>10</v>
-      </c>
-      <c r="C102" t="s">
-        <v>285</v>
-      </c>
-      <c r="D102" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" t="s">
-        <v>298</v>
+    <row r="102" spans="1:23" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G102" s="16"/>
       <c r="L102" s="16"/>
       <c r="Q102" s="16"/>
       <c r="V102" s="16"/>
-    </row>
-    <row r="103" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D103" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>299</v>
+      <c r="W102"/>
+    </row>
+    <row r="103" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>282</v>
+      </c>
+      <c r="B103" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103" t="s">
+        <v>283</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>296</v>
       </c>
       <c r="G103" s="16"/>
       <c r="L103" s="16"/>
       <c r="Q103" s="16"/>
       <c r="V103" s="16"/>
-      <c r="W103"/>
     </row>
     <row r="104" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>0</v>
@@ -4653,8 +4653,8 @@
       <c r="E104" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F104" s="2" t="s">
-        <v>16</v>
+      <c r="F104" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="G104" s="16"/>
       <c r="L104" s="16"/>
@@ -4662,21 +4662,24 @@
       <c r="V104" s="16"/>
       <c r="W104"/>
     </row>
-    <row r="105" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D105" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E105" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G105" s="16"/>
       <c r="L105" s="16"/>
@@ -4686,22 +4689,19 @@
     </row>
     <row r="106" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D106" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="G106" s="16"/>
       <c r="L106" s="16"/>
@@ -4709,15 +4709,15 @@
       <c r="V106" s="16"/>
       <c r="W106"/>
     </row>
-    <row r="107" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D107" s="2" t="b">
         <v>1</v>
@@ -4725,82 +4725,82 @@
       <c r="E107" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F107" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G107" s="16"/>
-      <c r="H107" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="L107" s="17"/>
-      <c r="M107" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="P107" s="2" t="s">
-        <v>326</v>
-      </c>
+      <c r="L107" s="16"/>
       <c r="Q107" s="16"/>
-      <c r="R107" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="S107" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="T107" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="U107" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="V107" s="16"/>
       <c r="W107"/>
     </row>
-    <row r="108" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D108" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>218</v>
+    <row r="108" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G108" s="16"/>
-      <c r="L108" s="16"/>
+      <c r="H108" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L108" s="17"/>
+      <c r="M108" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="N108" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="O108" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="P108" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="Q108" s="16"/>
+      <c r="R108" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="S108" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="T108" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="U108" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="V108" s="16"/>
       <c r="W108"/>
     </row>
     <row r="109" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D109" s="7" t="b">
         <v>1</v>
@@ -4819,22 +4819,22 @@
     </row>
     <row r="110" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D110" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E110" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="G110" s="16"/>
       <c r="L110" s="16"/>
@@ -4842,76 +4842,43 @@
       <c r="V110" s="16"/>
       <c r="W110"/>
     </row>
-    <row r="111" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B111" s="2" t="s">
+    <row r="111" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D111" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>1</v>
+      <c r="C111" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G111" s="16"/>
-      <c r="H111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K111" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L111" s="16"/>
-      <c r="M111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P111" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="Q111" s="16"/>
-      <c r="R111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U111" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="V111" s="16"/>
       <c r="W111"/>
     </row>
     <row r="112" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D112" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" s="2" t="b">
         <v>1</v>
@@ -4960,23 +4927,23 @@
     </row>
     <row r="113" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D113" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G113" s="16"/>
       <c r="H113" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>4</v>
@@ -4989,7 +4956,7 @@
       </c>
       <c r="L113" s="16"/>
       <c r="M113" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>4</v>
@@ -5002,7 +4969,7 @@
       </c>
       <c r="Q113" s="16"/>
       <c r="R113" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="S113" s="2" t="s">
         <v>4</v>
@@ -5016,15 +4983,15 @@
       <c r="V113" s="16"/>
       <c r="W113"/>
     </row>
-    <row r="114" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="D114" s="2" t="b">
         <v>0</v>
@@ -5032,36 +4999,65 @@
       <c r="E114" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F114" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G114" s="16"/>
-      <c r="H114"/>
-      <c r="I114"/>
-      <c r="J114"/>
-      <c r="K114"/>
+      <c r="H114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L114" s="16"/>
+      <c r="M114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="Q114" s="16"/>
+      <c r="R114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U114" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="V114" s="16"/>
       <c r="W114"/>
     </row>
-    <row r="115" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
-        <v>286</v>
-      </c>
-      <c r="B115" t="s">
+    <row r="115" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C115" t="s">
-        <v>287</v>
-      </c>
-      <c r="D115" t="b">
-        <v>0</v>
-      </c>
-      <c r="E115" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" t="s">
+      <c r="C115" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D115" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G115" s="16"/>
@@ -5070,107 +5066,79 @@
       <c r="J115"/>
       <c r="K115"/>
       <c r="L115" s="16"/>
-      <c r="M115"/>
-      <c r="N115"/>
-      <c r="O115"/>
-      <c r="P115"/>
       <c r="Q115" s="16"/>
-      <c r="R115"/>
-      <c r="S115"/>
-      <c r="T115"/>
-      <c r="U115"/>
       <c r="V115" s="16"/>
-    </row>
-    <row r="116" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A116" s="7" t="s">
+      <c r="W115"/>
+    </row>
+    <row r="116" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>284</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>285</v>
+      </c>
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" s="16"/>
+      <c r="H116"/>
+      <c r="I116"/>
+      <c r="J116"/>
+      <c r="K116"/>
+      <c r="L116" s="16"/>
+      <c r="M116"/>
+      <c r="N116"/>
+      <c r="O116"/>
+      <c r="P116"/>
+      <c r="Q116" s="16"/>
+      <c r="R116"/>
+      <c r="S116"/>
+      <c r="T116"/>
+      <c r="U116"/>
+      <c r="V116" s="16"/>
+    </row>
+    <row r="117" spans="1:23" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A117" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B117" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C117" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D116" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G116" s="16"/>
-      <c r="L116" s="16"/>
-      <c r="Q116" s="16"/>
-      <c r="V116" s="16"/>
-    </row>
-    <row r="117" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="2" t="b">
-        <v>1</v>
+      <c r="D117" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G117" s="16"/>
-      <c r="H117" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L117" s="16"/>
-      <c r="M117" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P117" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="Q117" s="16"/>
-      <c r="R117" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U117" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="V117" s="16"/>
     </row>
     <row r="118" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D118" s="2" t="b">
         <v>1</v>
@@ -5221,135 +5189,189 @@
     </row>
     <row r="119" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D119" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E119" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>298</v>
+        <v>1</v>
       </c>
       <c r="G119" s="16"/>
+      <c r="H119" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L119" s="16"/>
+      <c r="M119" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P119" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="Q119" s="16"/>
+      <c r="R119" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U119" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="V119" s="16"/>
     </row>
     <row r="120" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
-        <v>306</v>
+        <v>130</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G120" s="16"/>
+      <c r="L120" s="16"/>
+      <c r="Q120" s="16"/>
+      <c r="V120" s="16"/>
+    </row>
+    <row r="121" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G121" s="16"/>
+      <c r="H121" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="L121" s="17"/>
+      <c r="M121" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="O121" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="P121" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q121" s="16"/>
+      <c r="R121" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D120" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G120" s="16"/>
-      <c r="H120" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="I120" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="K120" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="L120" s="17"/>
-      <c r="M120" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="N120" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O120" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P120" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q120" s="16"/>
-      <c r="R120" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="S120" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="T120" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="U120" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="V120" s="16"/>
-    </row>
-    <row r="121" spans="1:23" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A121" s="2" t="s">
+      <c r="S121" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="T121" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="U121" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="V121" s="16"/>
+    </row>
+    <row r="122" spans="1:23" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A122" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D121" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E121" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="2" t="s">
+      <c r="D122" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="G121" s="16"/>
-      <c r="L121" s="16"/>
-      <c r="Q121" s="16"/>
-      <c r="V121" s="16"/>
-    </row>
-    <row r="122" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A122" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D122" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E122" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="G122" s="16"/>
       <c r="L122" s="16"/>
       <c r="Q122" s="16"/>
       <c r="V122" s="16"/>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="W123"/>
+    <row r="123" spans="1:23" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A123" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D123" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G123" s="16"/>
+      <c r="L123" s="16"/>
+      <c r="Q123" s="16"/>
+      <c r="V123" s="16"/>
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.4">
       <c r="W124"/>
@@ -5413,6 +5435,9 @@
     </row>
     <row r="144" spans="23:23" x14ac:dyDescent="0.4">
       <c r="W144"/>
+    </row>
+    <row r="145" spans="23:23" x14ac:dyDescent="0.4">
+      <c r="W145"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>